<commit_message>
Item and Quote Excel Changes
</commit_message>
<xml_diff>
--- a/NtierMvc/App_Data/Documents/Excel/QuotePreparation.xlsx
+++ b/NtierMvc/App_Data/Documents/Excel/QuotePreparation.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Deepak\Downloads\C#\NtierMvc\App_Data\Documents\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F3D8628-632C-4F68-A64D-9635D5F627A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8854AA02-2C26-4617-B815-110BC9EC12C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MOT F SM 08 Rev.00" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'MOT F SM 08 Rev.00'!$A$1:$H$38</definedName>
@@ -24,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="71">
   <si>
     <t>TERMS &amp; CONDITIONS</t>
   </si>
@@ -140,9 +139,6 @@
     <t>#OwnerSign</t>
   </si>
   <si>
-    <t>Total Weight  row deleted</t>
-  </si>
-  <si>
     <t>Quotation</t>
   </si>
   <si>
@@ -221,9 +217,6 @@
 (#Currency)</t>
   </si>
   <si>
-    <t>Amount In Words: To add</t>
-  </si>
-  <si>
     <t>Kamalakar Pathak</t>
   </si>
   <si>
@@ -287,19 +280,7 @@
     <t>Manufacturer</t>
   </si>
   <si>
-    <t>Added New Clause.  In case Type of Quote is Export then only show this clause</t>
-  </si>
-  <si>
     <t xml:space="preserve">Amount in Words: </t>
-  </si>
-  <si>
-    <t>Add itewise Delivery Time &amp; "Ex-Works"</t>
-  </si>
-  <si>
-    <t>Quotation Row moved here</t>
-  </si>
-  <si>
-    <t>To add Lead Time-Weeks &amp; Ex-works</t>
   </si>
 </sst>
 </file>
@@ -662,7 +643,7 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
@@ -796,8 +777,52 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -841,35 +866,23 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -892,38 +905,6 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
@@ -933,30 +914,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -980,6 +937,30 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -992,20 +973,24 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1415,8 +1400,8 @@
   </sheetPr>
   <dimension ref="A1:XFD43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:C9"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1429,302 +1414,298 @@
     <col min="6" max="6" width="19.28515625" style="1" customWidth="1"/>
     <col min="7" max="7" width="25.42578125" style="1" customWidth="1"/>
     <col min="8" max="8" width="26.85546875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="53"/>
-    <col min="10" max="10" width="9.140625" style="68"/>
-    <col min="11" max="16" width="9.140625" style="53"/>
+    <col min="9" max="9" width="9.140625" style="37"/>
+    <col min="10" max="10" width="9.140625" style="42"/>
+    <col min="11" max="16" width="9.140625" style="37"/>
     <col min="17" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16384" s="34" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="89" t="s">
+      <c r="A1" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="89"/>
-      <c r="C1" s="89"/>
-      <c r="D1" s="89"/>
-      <c r="E1" s="89"/>
-      <c r="F1" s="89"/>
-      <c r="G1" s="89"/>
-      <c r="H1" s="89"/>
-      <c r="I1" s="51"/>
-      <c r="J1" s="66"/>
-      <c r="K1" s="51"/>
-      <c r="L1" s="51"/>
-      <c r="M1" s="51"/>
-      <c r="N1" s="51"/>
-      <c r="O1" s="51"/>
-      <c r="P1" s="51"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="35"/>
+      <c r="L1" s="35"/>
+      <c r="M1" s="35"/>
+      <c r="N1" s="35"/>
+      <c r="O1" s="35"/>
+      <c r="P1" s="35"/>
     </row>
     <row r="2" spans="1:16384" s="4" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="55"/>
-      <c r="B2" s="60" t="s">
-        <v>40</v>
+      <c r="A2" s="65"/>
+      <c r="B2" s="62" t="s">
+        <v>39</v>
       </c>
-      <c r="C2" s="61"/>
-      <c r="D2" s="61"/>
-      <c r="E2" s="61"/>
-      <c r="F2" s="61"/>
-      <c r="G2" s="61"/>
-      <c r="H2" s="62"/>
-      <c r="J2" s="67"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="63"/>
+      <c r="F2" s="63"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="64"/>
+      <c r="J2" s="41"/>
     </row>
     <row r="3" spans="1:16384" s="4" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="56"/>
-      <c r="B3" s="57" t="s">
-        <v>39</v>
+      <c r="A3" s="66"/>
+      <c r="B3" s="67" t="s">
+        <v>38</v>
       </c>
-      <c r="C3" s="58"/>
-      <c r="D3" s="58"/>
-      <c r="E3" s="58"/>
-      <c r="F3" s="58"/>
-      <c r="G3" s="58"/>
-      <c r="H3" s="59"/>
-      <c r="J3" s="54" t="s">
-        <v>75</v>
-      </c>
+      <c r="C3" s="68"/>
+      <c r="D3" s="68"/>
+      <c r="E3" s="68"/>
+      <c r="F3" s="68"/>
+      <c r="G3" s="68"/>
+      <c r="H3" s="69"/>
+      <c r="J3" s="38"/>
     </row>
     <row r="4" spans="1:16384" s="4" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="36" t="s">
-        <v>43</v>
-      </c>
-      <c r="B4" s="36"/>
-      <c r="C4" s="36"/>
-      <c r="D4" s="35" t="s">
+      <c r="A4" s="50" t="s">
         <v>42</v>
       </c>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
+      <c r="B4" s="50"/>
+      <c r="C4" s="50"/>
+      <c r="D4" s="47" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
       <c r="G4" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="I4" s="52"/>
-      <c r="J4" s="54"/>
-      <c r="K4" s="52"/>
-      <c r="L4" s="52"/>
-      <c r="M4" s="52"/>
-      <c r="N4" s="52"/>
-      <c r="O4" s="52"/>
-      <c r="P4" s="52"/>
+      <c r="I4" s="36"/>
+      <c r="J4" s="38"/>
+      <c r="K4" s="36"/>
+      <c r="L4" s="36"/>
+      <c r="M4" s="36"/>
+      <c r="N4" s="36"/>
+      <c r="O4" s="36"/>
+      <c r="P4" s="36"/>
     </row>
     <row r="5" spans="1:16384" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="37"/>
-      <c r="B5" s="38"/>
-      <c r="C5" s="39"/>
-      <c r="D5" s="63" t="s">
-        <v>44</v>
+      <c r="A5" s="51"/>
+      <c r="B5" s="52"/>
+      <c r="C5" s="53"/>
+      <c r="D5" s="48" t="s">
+        <v>43</v>
       </c>
-      <c r="E5" s="64"/>
-      <c r="F5" s="64"/>
+      <c r="E5" s="49"/>
+      <c r="F5" s="49"/>
       <c r="G5" s="5" t="s">
         <v>6</v>
       </c>
       <c r="H5" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="I5" s="52"/>
-      <c r="J5" s="54"/>
-      <c r="K5" s="52"/>
-      <c r="L5" s="52"/>
-      <c r="M5" s="52"/>
-      <c r="N5" s="52"/>
-      <c r="O5" s="52"/>
-      <c r="P5" s="52"/>
+      <c r="I5" s="36"/>
+      <c r="J5" s="38"/>
+      <c r="K5" s="36"/>
+      <c r="L5" s="36"/>
+      <c r="M5" s="36"/>
+      <c r="N5" s="36"/>
+      <c r="O5" s="36"/>
+      <c r="P5" s="36"/>
     </row>
     <row r="6" spans="1:16384" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="40" t="s">
+      <c r="A6" s="54" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="41"/>
-      <c r="C6" s="42"/>
-      <c r="D6" s="63"/>
-      <c r="E6" s="64"/>
-      <c r="F6" s="64"/>
+      <c r="B6" s="55"/>
+      <c r="C6" s="56"/>
+      <c r="D6" s="48"/>
+      <c r="E6" s="49"/>
+      <c r="F6" s="49"/>
       <c r="G6" s="5" t="s">
         <v>7</v>
       </c>
       <c r="H6" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="I6" s="52"/>
-      <c r="J6" s="54"/>
-      <c r="K6" s="52"/>
-      <c r="L6" s="52"/>
-      <c r="M6" s="52"/>
-      <c r="N6" s="52"/>
-      <c r="O6" s="52"/>
-      <c r="P6" s="52"/>
+      <c r="I6" s="36"/>
+      <c r="J6" s="38"/>
+      <c r="K6" s="36"/>
+      <c r="L6" s="36"/>
+      <c r="M6" s="36"/>
+      <c r="N6" s="36"/>
+      <c r="O6" s="36"/>
+      <c r="P6" s="36"/>
     </row>
     <row r="7" spans="1:16384" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="40" t="s">
+      <c r="A7" s="54" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="41"/>
-      <c r="C7" s="42"/>
-      <c r="D7" s="63"/>
-      <c r="E7" s="64"/>
-      <c r="F7" s="64"/>
+      <c r="B7" s="55"/>
+      <c r="C7" s="56"/>
+      <c r="D7" s="48"/>
+      <c r="E7" s="49"/>
+      <c r="F7" s="49"/>
       <c r="G7" s="5" t="s">
         <v>17</v>
       </c>
       <c r="H7" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="I7" s="52"/>
-      <c r="J7" s="54"/>
-      <c r="K7" s="52"/>
-      <c r="L7" s="52"/>
-      <c r="M7" s="52"/>
-      <c r="N7" s="52"/>
-      <c r="O7" s="52"/>
-      <c r="P7" s="52"/>
+      <c r="I7" s="36"/>
+      <c r="J7" s="38"/>
+      <c r="K7" s="36"/>
+      <c r="L7" s="36"/>
+      <c r="M7" s="36"/>
+      <c r="N7" s="36"/>
+      <c r="O7" s="36"/>
+      <c r="P7" s="36"/>
     </row>
     <row r="8" spans="1:16384" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="40" t="s">
+      <c r="A8" s="54" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="41"/>
-      <c r="C8" s="42"/>
-      <c r="D8" s="63"/>
-      <c r="E8" s="64"/>
-      <c r="F8" s="64"/>
+      <c r="B8" s="55"/>
+      <c r="C8" s="56"/>
+      <c r="D8" s="48"/>
+      <c r="E8" s="49"/>
+      <c r="F8" s="49"/>
       <c r="G8" s="5" t="s">
         <v>19</v>
       </c>
       <c r="H8" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="I8" s="52"/>
-      <c r="J8" s="54"/>
-      <c r="K8" s="52"/>
-      <c r="L8" s="52"/>
-      <c r="M8" s="52"/>
-      <c r="N8" s="52"/>
-      <c r="O8" s="52"/>
-      <c r="P8" s="52"/>
+      <c r="I8" s="36"/>
+      <c r="J8" s="38"/>
+      <c r="K8" s="36"/>
+      <c r="L8" s="36"/>
+      <c r="M8" s="36"/>
+      <c r="N8" s="36"/>
+      <c r="O8" s="36"/>
+      <c r="P8" s="36"/>
     </row>
     <row r="9" spans="1:16384" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="40"/>
-      <c r="B9" s="41"/>
-      <c r="C9" s="42"/>
-      <c r="D9" s="63"/>
-      <c r="E9" s="64"/>
-      <c r="F9" s="64"/>
+      <c r="A9" s="54"/>
+      <c r="B9" s="55"/>
+      <c r="C9" s="56"/>
+      <c r="D9" s="48"/>
+      <c r="E9" s="49"/>
+      <c r="F9" s="49"/>
       <c r="G9" s="5" t="s">
         <v>5</v>
       </c>
       <c r="H9" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="I9" s="52"/>
-      <c r="J9" s="54"/>
-      <c r="K9" s="52"/>
-      <c r="L9" s="52"/>
-      <c r="M9" s="52"/>
-      <c r="N9" s="52"/>
-      <c r="O9" s="52"/>
-      <c r="P9" s="52"/>
+      <c r="I9" s="36"/>
+      <c r="J9" s="38"/>
+      <c r="K9" s="36"/>
+      <c r="L9" s="36"/>
+      <c r="M9" s="36"/>
+      <c r="N9" s="36"/>
+      <c r="O9" s="36"/>
+      <c r="P9" s="36"/>
     </row>
     <row r="10" spans="1:16384" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="40"/>
-      <c r="B10" s="41"/>
-      <c r="C10" s="42"/>
-      <c r="D10" s="63"/>
-      <c r="E10" s="64"/>
-      <c r="F10" s="64"/>
+      <c r="A10" s="54"/>
+      <c r="B10" s="55"/>
+      <c r="C10" s="56"/>
+      <c r="D10" s="48"/>
+      <c r="E10" s="49"/>
+      <c r="F10" s="49"/>
       <c r="G10" s="5" t="s">
         <v>4</v>
       </c>
       <c r="H10" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="I10" s="52"/>
-      <c r="J10" s="65" t="s">
-        <v>38</v>
-      </c>
-      <c r="K10" s="52"/>
-      <c r="L10" s="52"/>
-      <c r="M10" s="52"/>
-      <c r="N10" s="52"/>
-      <c r="O10" s="52"/>
-      <c r="P10" s="52"/>
+      <c r="I10" s="36"/>
+      <c r="J10" s="39"/>
+      <c r="K10" s="36"/>
+      <c r="L10" s="36"/>
+      <c r="M10" s="36"/>
+      <c r="N10" s="36"/>
+      <c r="O10" s="36"/>
+      <c r="P10" s="36"/>
     </row>
     <row r="11" spans="1:16384" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="43"/>
-      <c r="B11" s="44"/>
-      <c r="C11" s="45"/>
-      <c r="D11" s="63"/>
-      <c r="E11" s="64"/>
-      <c r="F11" s="64"/>
+      <c r="A11" s="57"/>
+      <c r="B11" s="58"/>
+      <c r="C11" s="59"/>
+      <c r="D11" s="48"/>
+      <c r="E11" s="49"/>
+      <c r="F11" s="49"/>
       <c r="G11" s="5" t="s">
         <v>11</v>
       </c>
       <c r="H11" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="I11" s="52"/>
-      <c r="J11" s="67"/>
-      <c r="K11" s="52"/>
-      <c r="L11" s="52"/>
-      <c r="M11" s="52"/>
-      <c r="N11" s="52"/>
-      <c r="O11" s="52"/>
-      <c r="P11" s="52"/>
+      <c r="I11" s="36"/>
+      <c r="J11" s="41"/>
+      <c r="K11" s="36"/>
+      <c r="L11" s="36"/>
+      <c r="M11" s="36"/>
+      <c r="N11" s="36"/>
+      <c r="O11" s="36"/>
+      <c r="P11" s="36"/>
     </row>
     <row r="12" spans="1:16384" s="4" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="35" t="s">
+      <c r="A12" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="35"/>
-      <c r="C12" s="35"/>
-      <c r="D12" s="35"/>
-      <c r="E12" s="35"/>
-      <c r="F12" s="35"/>
-      <c r="G12" s="35"/>
-      <c r="H12" s="35"/>
-      <c r="I12" s="52"/>
-      <c r="K12" s="52"/>
-      <c r="L12" s="52"/>
-      <c r="M12" s="52"/>
-      <c r="N12" s="52"/>
-      <c r="O12" s="52"/>
-      <c r="P12" s="52"/>
+      <c r="B12" s="47"/>
+      <c r="C12" s="47"/>
+      <c r="D12" s="47"/>
+      <c r="E12" s="47"/>
+      <c r="F12" s="47"/>
+      <c r="G12" s="47"/>
+      <c r="H12" s="47"/>
+      <c r="I12" s="36"/>
+      <c r="K12" s="36"/>
+      <c r="L12" s="36"/>
+      <c r="M12" s="36"/>
+      <c r="N12" s="36"/>
+      <c r="O12" s="36"/>
+      <c r="P12" s="36"/>
     </row>
     <row r="13" spans="1:16384" s="13" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>8</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D13" s="11" t="s">
         <v>9</v>
       </c>
       <c r="E13" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="F13" s="12" t="s">
+      <c r="G13" s="12" t="s">
         <v>48</v>
-      </c>
-      <c r="G13" s="12" t="s">
-        <v>49</v>
       </c>
       <c r="H13" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="I13" s="52"/>
-      <c r="J13" s="54"/>
-      <c r="K13" s="52"/>
-      <c r="L13" s="52"/>
-      <c r="M13" s="52"/>
-      <c r="N13" s="52"/>
-      <c r="O13" s="52"/>
-      <c r="P13" s="52"/>
+      <c r="I13" s="36"/>
+      <c r="J13" s="38"/>
+      <c r="K13" s="36"/>
+      <c r="L13" s="36"/>
+      <c r="M13" s="36"/>
+      <c r="N13" s="36"/>
+      <c r="O13" s="36"/>
+      <c r="P13" s="36"/>
       <c r="Q13" s="4"/>
       <c r="R13" s="4"/>
       <c r="S13" s="4"/>
@@ -18095,7 +18076,7 @@
       <c r="XFD13" s="4"/>
     </row>
     <row r="14" spans="1:16384" s="13" customFormat="1" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A14" s="14"/>
+      <c r="A14" s="90"/>
       <c r="B14" s="14"/>
       <c r="C14" s="15"/>
       <c r="D14" s="16"/>
@@ -18103,16 +18084,14 @@
       <c r="F14" s="17"/>
       <c r="G14" s="17"/>
       <c r="H14" s="14"/>
-      <c r="I14" s="52"/>
-      <c r="J14" s="54" t="s">
-        <v>74</v>
-      </c>
-      <c r="K14" s="52"/>
-      <c r="L14" s="52"/>
-      <c r="M14" s="52"/>
-      <c r="N14" s="52"/>
-      <c r="O14" s="52"/>
-      <c r="P14" s="52"/>
+      <c r="I14" s="36"/>
+      <c r="J14" s="38"/>
+      <c r="K14" s="36"/>
+      <c r="L14" s="36"/>
+      <c r="M14" s="36"/>
+      <c r="N14" s="36"/>
+      <c r="O14" s="36"/>
+      <c r="P14" s="36"/>
       <c r="Q14" s="4"/>
       <c r="R14" s="4"/>
       <c r="S14" s="4"/>
@@ -34483,7 +34462,7 @@
       <c r="XFD14" s="4"/>
     </row>
     <row r="15" spans="1:16384" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="18"/>
+      <c r="A15" s="91"/>
       <c r="B15" s="18"/>
       <c r="C15" s="19"/>
       <c r="D15" s="18"/>
@@ -34505,469 +34484,463 @@
         <v>33</v>
       </c>
       <c r="H16" s="28"/>
-      <c r="I16" s="54"/>
-      <c r="J16" s="54"/>
-      <c r="K16" s="54"/>
-      <c r="L16" s="54"/>
-      <c r="M16" s="54"/>
-      <c r="N16" s="54"/>
-      <c r="O16" s="54"/>
-      <c r="P16" s="54"/>
+      <c r="I16" s="38"/>
+      <c r="J16" s="38"/>
+      <c r="K16" s="38"/>
+      <c r="L16" s="38"/>
+      <c r="M16" s="38"/>
+      <c r="N16" s="38"/>
+      <c r="O16" s="38"/>
+      <c r="P16" s="38"/>
     </row>
     <row r="17" spans="1:16" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="80" t="s">
-        <v>73</v>
+      <c r="A17" s="75" t="s">
+        <v>70</v>
       </c>
-      <c r="B17" s="81"/>
-      <c r="C17" s="81"/>
-      <c r="D17" s="81"/>
-      <c r="E17" s="81"/>
-      <c r="F17" s="81"/>
-      <c r="G17" s="81"/>
-      <c r="H17" s="82"/>
-      <c r="J17" s="54" t="s">
+      <c r="B17" s="76"/>
+      <c r="C17" s="76"/>
+      <c r="D17" s="76"/>
+      <c r="E17" s="76"/>
+      <c r="F17" s="76"/>
+      <c r="G17" s="76"/>
+      <c r="H17" s="77"/>
+      <c r="J17" s="38"/>
+      <c r="K17" s="36"/>
+      <c r="L17" s="36"/>
+      <c r="M17" s="36"/>
+      <c r="N17" s="36"/>
+      <c r="O17" s="36"/>
+      <c r="P17" s="36"/>
+    </row>
+    <row r="18" spans="1:16" s="2" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="70" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="71"/>
+      <c r="C18" s="71"/>
+      <c r="D18" s="71"/>
+      <c r="E18" s="71"/>
+      <c r="F18" s="71"/>
+      <c r="G18" s="71"/>
+      <c r="H18" s="72"/>
+      <c r="I18" s="36"/>
+      <c r="J18" s="38"/>
+      <c r="K18" s="36"/>
+      <c r="L18" s="36"/>
+      <c r="M18" s="36"/>
+      <c r="N18" s="36"/>
+      <c r="O18" s="36"/>
+      <c r="P18" s="36"/>
+    </row>
+    <row r="19" spans="1:16" s="2" customFormat="1" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="73" t="s">
+        <v>57</v>
+      </c>
+      <c r="B19" s="74"/>
+      <c r="C19" s="61" t="s">
+        <v>36</v>
+      </c>
+      <c r="D19" s="61"/>
+      <c r="E19" s="61"/>
+      <c r="F19" s="61"/>
+      <c r="G19" s="61"/>
+      <c r="H19" s="61"/>
+      <c r="I19" s="36"/>
+      <c r="J19" s="38"/>
+      <c r="K19" s="36"/>
+      <c r="L19" s="36"/>
+      <c r="M19" s="36"/>
+      <c r="N19" s="36"/>
+      <c r="O19" s="36"/>
+      <c r="P19" s="36"/>
+    </row>
+    <row r="20" spans="1:16" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="73" t="s">
+        <v>58</v>
+      </c>
+      <c r="B20" s="74"/>
+      <c r="C20" s="60"/>
+      <c r="D20" s="60"/>
+      <c r="E20" s="60"/>
+      <c r="F20" s="60"/>
+      <c r="G20" s="60"/>
+      <c r="H20" s="60"/>
+      <c r="I20" s="36"/>
+      <c r="J20" s="38"/>
+      <c r="K20" s="36"/>
+      <c r="L20" s="36"/>
+      <c r="M20" s="36"/>
+      <c r="N20" s="36"/>
+      <c r="O20" s="36"/>
+      <c r="P20" s="36"/>
+    </row>
+    <row r="21" spans="1:16" s="2" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="73" t="s">
+        <v>59</v>
+      </c>
+      <c r="B21" s="74"/>
+      <c r="C21" s="60" t="s">
+        <v>35</v>
+      </c>
+      <c r="D21" s="60"/>
+      <c r="E21" s="60"/>
+      <c r="F21" s="60"/>
+      <c r="G21" s="60"/>
+      <c r="H21" s="60"/>
+      <c r="I21" s="36"/>
+      <c r="J21" s="38"/>
+      <c r="K21" s="36"/>
+      <c r="L21" s="36"/>
+      <c r="M21" s="36"/>
+      <c r="N21" s="36"/>
+      <c r="O21" s="36"/>
+      <c r="P21" s="36"/>
+    </row>
+    <row r="22" spans="1:16" s="2" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="73" t="s">
+        <v>60</v>
+      </c>
+      <c r="B22" s="74"/>
+      <c r="C22" s="60" t="s">
+        <v>30</v>
+      </c>
+      <c r="D22" s="60"/>
+      <c r="E22" s="60"/>
+      <c r="F22" s="60"/>
+      <c r="G22" s="60"/>
+      <c r="H22" s="60"/>
+      <c r="I22" s="36"/>
+      <c r="J22" s="38"/>
+      <c r="K22" s="36"/>
+      <c r="L22" s="36"/>
+      <c r="M22" s="36"/>
+      <c r="N22" s="36"/>
+      <c r="O22" s="36"/>
+      <c r="P22" s="36"/>
+    </row>
+    <row r="23" spans="1:16" s="2" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="73" t="s">
+        <v>61</v>
+      </c>
+      <c r="B23" s="74"/>
+      <c r="C23" s="61" t="s">
+        <v>51</v>
+      </c>
+      <c r="D23" s="61"/>
+      <c r="E23" s="61"/>
+      <c r="F23" s="61"/>
+      <c r="G23" s="61"/>
+      <c r="H23" s="61"/>
+      <c r="I23" s="36"/>
+      <c r="J23" s="38"/>
+      <c r="K23" s="36"/>
+      <c r="L23" s="36"/>
+      <c r="M23" s="36"/>
+      <c r="N23" s="36"/>
+      <c r="O23" s="36"/>
+      <c r="P23" s="36"/>
+    </row>
+    <row r="24" spans="1:16" s="2" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="73" t="s">
+        <v>62</v>
+      </c>
+      <c r="B24" s="74"/>
+      <c r="C24" s="60" t="s">
+        <v>12</v>
+      </c>
+      <c r="D24" s="60"/>
+      <c r="E24" s="60"/>
+      <c r="F24" s="60"/>
+      <c r="G24" s="60"/>
+      <c r="H24" s="60"/>
+      <c r="I24" s="36"/>
+      <c r="J24" s="38"/>
+      <c r="K24" s="36"/>
+      <c r="L24" s="36"/>
+      <c r="M24" s="36"/>
+      <c r="N24" s="36"/>
+      <c r="O24" s="36"/>
+      <c r="P24" s="36"/>
+    </row>
+    <row r="25" spans="1:16" s="2" customFormat="1" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A25" s="73" t="s">
+        <v>63</v>
+      </c>
+      <c r="B25" s="74"/>
+      <c r="C25" s="60" t="s">
+        <v>34</v>
+      </c>
+      <c r="D25" s="60"/>
+      <c r="E25" s="60"/>
+      <c r="F25" s="60"/>
+      <c r="G25" s="60"/>
+      <c r="H25" s="60"/>
+      <c r="I25" s="36"/>
+      <c r="J25" s="38"/>
+      <c r="K25" s="36"/>
+      <c r="L25" s="36"/>
+      <c r="M25" s="36"/>
+      <c r="N25" s="36"/>
+      <c r="O25" s="36"/>
+      <c r="P25" s="36"/>
+    </row>
+    <row r="26" spans="1:16" s="2" customFormat="1" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A26" s="73" t="s">
+        <v>64</v>
+      </c>
+      <c r="B26" s="74"/>
+      <c r="C26" s="61" t="s">
+        <v>13</v>
+      </c>
+      <c r="D26" s="61"/>
+      <c r="E26" s="61"/>
+      <c r="F26" s="61"/>
+      <c r="G26" s="61"/>
+      <c r="H26" s="61"/>
+      <c r="I26" s="36"/>
+      <c r="J26" s="38"/>
+      <c r="K26" s="36"/>
+      <c r="L26" s="36"/>
+      <c r="M26" s="36"/>
+      <c r="N26" s="36"/>
+      <c r="O26" s="36"/>
+      <c r="P26" s="36"/>
+    </row>
+    <row r="27" spans="1:16" s="2" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="73" t="s">
+        <v>65</v>
+      </c>
+      <c r="B27" s="74"/>
+      <c r="C27" s="60" t="s">
+        <v>14</v>
+      </c>
+      <c r="D27" s="60"/>
+      <c r="E27" s="60"/>
+      <c r="F27" s="60"/>
+      <c r="G27" s="60"/>
+      <c r="H27" s="60"/>
+      <c r="I27" s="36"/>
+      <c r="J27" s="38"/>
+      <c r="K27" s="36"/>
+      <c r="L27" s="36"/>
+      <c r="M27" s="36"/>
+      <c r="N27" s="36"/>
+      <c r="O27" s="36"/>
+      <c r="P27" s="36"/>
+    </row>
+    <row r="28" spans="1:16" s="2" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="73" t="s">
+        <v>52</v>
+      </c>
+      <c r="B28" s="74"/>
+      <c r="C28" s="84" t="s">
+        <v>53</v>
+      </c>
+      <c r="D28" s="85"/>
+      <c r="E28" s="85"/>
+      <c r="F28" s="85"/>
+      <c r="G28" s="85"/>
+      <c r="H28" s="86"/>
+      <c r="J28" s="38"/>
+      <c r="K28" s="36"/>
+      <c r="L28" s="36"/>
+      <c r="M28" s="36"/>
+      <c r="N28" s="36"/>
+      <c r="O28" s="36"/>
+      <c r="P28" s="36"/>
+    </row>
+    <row r="29" spans="1:16" s="2" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="73" t="s">
+        <v>66</v>
+      </c>
+      <c r="B29" s="74"/>
+      <c r="C29" s="61" t="s">
+        <v>15</v>
+      </c>
+      <c r="D29" s="61"/>
+      <c r="E29" s="61"/>
+      <c r="F29" s="61"/>
+      <c r="G29" s="61"/>
+      <c r="H29" s="61"/>
+      <c r="I29" s="36"/>
+      <c r="K29" s="36"/>
+      <c r="L29" s="36"/>
+      <c r="M29" s="36"/>
+      <c r="N29" s="36"/>
+      <c r="O29" s="36"/>
+      <c r="P29" s="36"/>
+    </row>
+    <row r="30" spans="1:16" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="73" t="s">
+        <v>67</v>
+      </c>
+      <c r="B30" s="74"/>
+      <c r="C30" s="60" t="s">
+        <v>54</v>
+      </c>
+      <c r="D30" s="60"/>
+      <c r="E30" s="60"/>
+      <c r="F30" s="60"/>
+      <c r="G30" s="60"/>
+      <c r="H30" s="60"/>
+      <c r="I30" s="36"/>
+      <c r="J30" s="38"/>
+      <c r="K30" s="36"/>
+      <c r="L30" s="36"/>
+      <c r="M30" s="36"/>
+      <c r="N30" s="36"/>
+      <c r="O30" s="36"/>
+      <c r="P30" s="36"/>
+    </row>
+    <row r="31" spans="1:16" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="73" t="s">
+        <v>68</v>
+      </c>
+      <c r="B31" s="74"/>
+      <c r="C31" s="60" t="s">
+        <v>16</v>
+      </c>
+      <c r="D31" s="60"/>
+      <c r="E31" s="60"/>
+      <c r="F31" s="60"/>
+      <c r="G31" s="60"/>
+      <c r="H31" s="60"/>
+      <c r="I31" s="36"/>
+      <c r="J31" s="38"/>
+      <c r="K31" s="36"/>
+      <c r="L31" s="36"/>
+      <c r="M31" s="36"/>
+      <c r="N31" s="36"/>
+      <c r="O31" s="36"/>
+      <c r="P31" s="36"/>
+    </row>
+    <row r="32" spans="1:16" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="73" t="s">
+        <v>56</v>
+      </c>
+      <c r="B32" s="74"/>
+      <c r="C32" s="60" t="s">
+        <v>1</v>
+      </c>
+      <c r="D32" s="60"/>
+      <c r="E32" s="60"/>
+      <c r="F32" s="60"/>
+      <c r="G32" s="60"/>
+      <c r="H32" s="60"/>
+      <c r="I32" s="36"/>
+      <c r="J32" s="38"/>
+      <c r="K32" s="36"/>
+      <c r="L32" s="36"/>
+      <c r="M32" s="36"/>
+      <c r="N32" s="36"/>
+      <c r="O32" s="36"/>
+      <c r="P32" s="36"/>
+    </row>
+    <row r="33" spans="1:16" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="73" t="s">
+        <v>69</v>
+      </c>
+      <c r="B33" s="74"/>
+      <c r="C33" s="60" t="s">
+        <v>55</v>
+      </c>
+      <c r="D33" s="60"/>
+      <c r="E33" s="60"/>
+      <c r="F33" s="60"/>
+      <c r="G33" s="60"/>
+      <c r="H33" s="60"/>
+      <c r="I33" s="36"/>
+      <c r="J33" s="38"/>
+      <c r="K33" s="36"/>
+      <c r="L33" s="36"/>
+      <c r="M33" s="36"/>
+      <c r="N33" s="36"/>
+      <c r="O33" s="36"/>
+      <c r="P33" s="36"/>
+    </row>
+    <row r="34" spans="1:16" s="2" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="43" t="s">
+        <v>37</v>
+      </c>
+      <c r="B34" s="44"/>
+      <c r="C34" s="44"/>
+      <c r="D34" s="44"/>
+      <c r="E34" s="44"/>
+      <c r="F34" s="44"/>
+      <c r="G34" s="44"/>
+      <c r="H34" s="45"/>
+      <c r="I34" s="36"/>
+      <c r="J34" s="38"/>
+      <c r="K34" s="36"/>
+      <c r="L34" s="36"/>
+      <c r="M34" s="36"/>
+      <c r="N34" s="36"/>
+      <c r="O34" s="36"/>
+      <c r="P34" s="36"/>
+    </row>
+    <row r="35" spans="1:16" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="87" t="s">
+        <v>49</v>
+      </c>
+      <c r="B35" s="88"/>
+      <c r="C35" s="88"/>
+      <c r="D35" s="88"/>
+      <c r="E35" s="88"/>
+      <c r="F35" s="88"/>
+      <c r="G35" s="88"/>
+      <c r="H35" s="89"/>
+      <c r="I35" s="36"/>
+      <c r="J35" s="38"/>
+      <c r="K35" s="36"/>
+      <c r="L35" s="36"/>
+      <c r="M35" s="36"/>
+      <c r="N35" s="36"/>
+      <c r="O35" s="36"/>
+      <c r="P35" s="36"/>
+    </row>
+    <row r="36" spans="1:16" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="78" t="s">
         <v>50</v>
       </c>
-      <c r="K17" s="52"/>
-      <c r="L17" s="52"/>
-      <c r="M17" s="52"/>
-      <c r="N17" s="52"/>
-      <c r="O17" s="52"/>
-      <c r="P17" s="52"/>
-    </row>
-    <row r="18" spans="1:16" s="2" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="69" t="s">
-        <v>0</v>
-      </c>
-      <c r="B18" s="70"/>
-      <c r="C18" s="70"/>
-      <c r="D18" s="70"/>
-      <c r="E18" s="70"/>
-      <c r="F18" s="70"/>
-      <c r="G18" s="70"/>
-      <c r="H18" s="71"/>
-      <c r="I18" s="52"/>
-      <c r="J18" s="54"/>
-      <c r="K18" s="52"/>
-      <c r="L18" s="52"/>
-      <c r="M18" s="52"/>
-      <c r="N18" s="52"/>
-      <c r="O18" s="52"/>
-      <c r="P18" s="52"/>
-    </row>
-    <row r="19" spans="1:16" s="2" customFormat="1" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="78" t="s">
-        <v>59</v>
-      </c>
-      <c r="B19" s="79"/>
-      <c r="C19" s="46" t="s">
-        <v>36</v>
-      </c>
-      <c r="D19" s="46"/>
-      <c r="E19" s="46"/>
-      <c r="F19" s="46"/>
-      <c r="G19" s="46"/>
-      <c r="H19" s="46"/>
-      <c r="I19" s="52"/>
-      <c r="J19" s="54"/>
-      <c r="K19" s="52"/>
-      <c r="L19" s="52"/>
-      <c r="M19" s="52"/>
-      <c r="N19" s="52"/>
-      <c r="O19" s="52"/>
-      <c r="P19" s="52"/>
-    </row>
-    <row r="20" spans="1:16" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="78" t="s">
-        <v>60</v>
-      </c>
-      <c r="B20" s="79"/>
-      <c r="C20" s="47"/>
-      <c r="D20" s="47"/>
-      <c r="E20" s="47"/>
-      <c r="F20" s="47"/>
-      <c r="G20" s="47"/>
-      <c r="H20" s="47"/>
-      <c r="I20" s="52"/>
-      <c r="J20" s="54" t="s">
-        <v>76</v>
-      </c>
-      <c r="K20" s="52"/>
-      <c r="L20" s="52"/>
-      <c r="M20" s="52"/>
-      <c r="N20" s="52"/>
-      <c r="O20" s="52"/>
-      <c r="P20" s="52"/>
-    </row>
-    <row r="21" spans="1:16" s="2" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="78" t="s">
-        <v>61</v>
-      </c>
-      <c r="B21" s="79"/>
-      <c r="C21" s="47" t="s">
-        <v>35</v>
-      </c>
-      <c r="D21" s="47"/>
-      <c r="E21" s="47"/>
-      <c r="F21" s="47"/>
-      <c r="G21" s="47"/>
-      <c r="H21" s="47"/>
-      <c r="I21" s="52"/>
-      <c r="J21" s="54"/>
-      <c r="K21" s="52"/>
-      <c r="L21" s="52"/>
-      <c r="M21" s="52"/>
-      <c r="N21" s="52"/>
-      <c r="O21" s="52"/>
-      <c r="P21" s="52"/>
-    </row>
-    <row r="22" spans="1:16" s="2" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="78" t="s">
-        <v>62</v>
-      </c>
-      <c r="B22" s="79"/>
-      <c r="C22" s="47" t="s">
-        <v>30</v>
-      </c>
-      <c r="D22" s="47"/>
-      <c r="E22" s="47"/>
-      <c r="F22" s="47"/>
-      <c r="G22" s="47"/>
-      <c r="H22" s="47"/>
-      <c r="I22" s="52"/>
-      <c r="J22" s="54"/>
-      <c r="K22" s="52"/>
-      <c r="L22" s="52"/>
-      <c r="M22" s="52"/>
-      <c r="N22" s="52"/>
-      <c r="O22" s="52"/>
-      <c r="P22" s="52"/>
-    </row>
-    <row r="23" spans="1:16" s="2" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="78" t="s">
-        <v>63</v>
-      </c>
-      <c r="B23" s="79"/>
-      <c r="C23" s="46" t="s">
-        <v>53</v>
-      </c>
-      <c r="D23" s="46"/>
-      <c r="E23" s="46"/>
-      <c r="F23" s="46"/>
-      <c r="G23" s="46"/>
-      <c r="H23" s="46"/>
-      <c r="I23" s="52"/>
-      <c r="J23" s="54"/>
-      <c r="K23" s="52"/>
-      <c r="L23" s="52"/>
-      <c r="M23" s="52"/>
-      <c r="N23" s="52"/>
-      <c r="O23" s="52"/>
-      <c r="P23" s="52"/>
-    </row>
-    <row r="24" spans="1:16" s="2" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="78" t="s">
-        <v>64</v>
-      </c>
-      <c r="B24" s="79"/>
-      <c r="C24" s="47" t="s">
-        <v>12</v>
-      </c>
-      <c r="D24" s="47"/>
-      <c r="E24" s="47"/>
-      <c r="F24" s="47"/>
-      <c r="G24" s="47"/>
-      <c r="H24" s="47"/>
-      <c r="I24" s="52"/>
-      <c r="J24" s="54"/>
-      <c r="K24" s="52"/>
-      <c r="L24" s="52"/>
-      <c r="M24" s="52"/>
-      <c r="N24" s="52"/>
-      <c r="O24" s="52"/>
-      <c r="P24" s="52"/>
-    </row>
-    <row r="25" spans="1:16" s="2" customFormat="1" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A25" s="78" t="s">
-        <v>65</v>
-      </c>
-      <c r="B25" s="79"/>
-      <c r="C25" s="47" t="s">
-        <v>34</v>
-      </c>
-      <c r="D25" s="47"/>
-      <c r="E25" s="47"/>
-      <c r="F25" s="47"/>
-      <c r="G25" s="47"/>
-      <c r="H25" s="47"/>
-      <c r="I25" s="52"/>
-      <c r="J25" s="54"/>
-      <c r="K25" s="52"/>
-      <c r="L25" s="52"/>
-      <c r="M25" s="52"/>
-      <c r="N25" s="52"/>
-      <c r="O25" s="52"/>
-      <c r="P25" s="52"/>
-    </row>
-    <row r="26" spans="1:16" s="2" customFormat="1" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A26" s="78" t="s">
-        <v>66</v>
-      </c>
-      <c r="B26" s="79"/>
-      <c r="C26" s="46" t="s">
-        <v>13</v>
-      </c>
-      <c r="D26" s="46"/>
-      <c r="E26" s="46"/>
-      <c r="F26" s="46"/>
-      <c r="G26" s="46"/>
-      <c r="H26" s="46"/>
-      <c r="I26" s="52"/>
-      <c r="J26" s="54"/>
-      <c r="K26" s="52"/>
-      <c r="L26" s="52"/>
-      <c r="M26" s="52"/>
-      <c r="N26" s="52"/>
-      <c r="O26" s="52"/>
-      <c r="P26" s="52"/>
-    </row>
-    <row r="27" spans="1:16" s="2" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="78" t="s">
-        <v>67</v>
-      </c>
-      <c r="B27" s="79"/>
-      <c r="C27" s="47" t="s">
-        <v>14</v>
-      </c>
-      <c r="D27" s="47"/>
-      <c r="E27" s="47"/>
-      <c r="F27" s="47"/>
-      <c r="G27" s="47"/>
-      <c r="H27" s="47"/>
-      <c r="I27" s="52"/>
-      <c r="J27" s="54"/>
-      <c r="K27" s="52"/>
-      <c r="L27" s="52"/>
-      <c r="M27" s="52"/>
-      <c r="N27" s="52"/>
-      <c r="O27" s="52"/>
-      <c r="P27" s="52"/>
-    </row>
-    <row r="28" spans="1:16" s="2" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="78" t="s">
-        <v>54</v>
-      </c>
-      <c r="B28" s="79"/>
-      <c r="C28" s="83" t="s">
-        <v>55</v>
-      </c>
-      <c r="D28" s="84"/>
-      <c r="E28" s="84"/>
-      <c r="F28" s="84"/>
-      <c r="G28" s="84"/>
-      <c r="H28" s="85"/>
-      <c r="J28" s="54" t="s">
-        <v>72</v>
-      </c>
-      <c r="K28" s="52"/>
-      <c r="L28" s="52"/>
-      <c r="M28" s="52"/>
-      <c r="N28" s="52"/>
-      <c r="O28" s="52"/>
-      <c r="P28" s="52"/>
-    </row>
-    <row r="29" spans="1:16" s="2" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="78" t="s">
-        <v>68</v>
-      </c>
-      <c r="B29" s="79"/>
-      <c r="C29" s="46" t="s">
-        <v>15</v>
-      </c>
-      <c r="D29" s="46"/>
-      <c r="E29" s="46"/>
-      <c r="F29" s="46"/>
-      <c r="G29" s="46"/>
-      <c r="H29" s="46"/>
-      <c r="I29" s="52"/>
-      <c r="K29" s="52"/>
-      <c r="L29" s="52"/>
-      <c r="M29" s="52"/>
-      <c r="N29" s="52"/>
-      <c r="O29" s="52"/>
-      <c r="P29" s="52"/>
-    </row>
-    <row r="30" spans="1:16" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="78" t="s">
-        <v>69</v>
-      </c>
-      <c r="B30" s="79"/>
-      <c r="C30" s="47" t="s">
-        <v>56</v>
-      </c>
-      <c r="D30" s="47"/>
-      <c r="E30" s="47"/>
-      <c r="F30" s="47"/>
-      <c r="G30" s="47"/>
-      <c r="H30" s="47"/>
-      <c r="I30" s="52"/>
-      <c r="J30" s="54"/>
-      <c r="K30" s="52"/>
-      <c r="L30" s="52"/>
-      <c r="M30" s="52"/>
-      <c r="N30" s="52"/>
-      <c r="O30" s="52"/>
-      <c r="P30" s="52"/>
-    </row>
-    <row r="31" spans="1:16" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="78" t="s">
-        <v>70</v>
-      </c>
-      <c r="B31" s="79"/>
-      <c r="C31" s="47" t="s">
-        <v>16</v>
-      </c>
-      <c r="D31" s="47"/>
-      <c r="E31" s="47"/>
-      <c r="F31" s="47"/>
-      <c r="G31" s="47"/>
-      <c r="H31" s="47"/>
-      <c r="I31" s="52"/>
-      <c r="J31" s="54"/>
-      <c r="K31" s="52"/>
-      <c r="L31" s="52"/>
-      <c r="M31" s="52"/>
-      <c r="N31" s="52"/>
-      <c r="O31" s="52"/>
-      <c r="P31" s="52"/>
-    </row>
-    <row r="32" spans="1:16" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="78" t="s">
-        <v>58</v>
-      </c>
-      <c r="B32" s="79"/>
-      <c r="C32" s="47" t="s">
-        <v>1</v>
-      </c>
-      <c r="D32" s="47"/>
-      <c r="E32" s="47"/>
-      <c r="F32" s="47"/>
-      <c r="G32" s="47"/>
-      <c r="H32" s="47"/>
-      <c r="I32" s="52"/>
-      <c r="J32" s="54"/>
-      <c r="K32" s="52"/>
-      <c r="L32" s="52"/>
-      <c r="M32" s="52"/>
-      <c r="N32" s="52"/>
-      <c r="O32" s="52"/>
-      <c r="P32" s="52"/>
-    </row>
-    <row r="33" spans="1:16" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="78" t="s">
-        <v>71</v>
-      </c>
-      <c r="B33" s="79"/>
-      <c r="C33" s="47" t="s">
-        <v>57</v>
-      </c>
-      <c r="D33" s="47"/>
-      <c r="E33" s="47"/>
-      <c r="F33" s="47"/>
-      <c r="G33" s="47"/>
-      <c r="H33" s="47"/>
-      <c r="I33" s="52"/>
-      <c r="J33" s="54"/>
-      <c r="K33" s="52"/>
-      <c r="L33" s="52"/>
-      <c r="M33" s="52"/>
-      <c r="N33" s="52"/>
-      <c r="O33" s="52"/>
-      <c r="P33" s="52"/>
-    </row>
-    <row r="34" spans="1:16" s="2" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="86" t="s">
-        <v>37</v>
-      </c>
-      <c r="B34" s="87"/>
-      <c r="C34" s="87"/>
-      <c r="D34" s="87"/>
-      <c r="E34" s="87"/>
-      <c r="F34" s="87"/>
-      <c r="G34" s="87"/>
-      <c r="H34" s="88"/>
-      <c r="I34" s="52"/>
-      <c r="J34" s="54"/>
-      <c r="K34" s="52"/>
-      <c r="L34" s="52"/>
-      <c r="M34" s="52"/>
-      <c r="N34" s="52"/>
-      <c r="O34" s="52"/>
-      <c r="P34" s="52"/>
-    </row>
-    <row r="35" spans="1:16" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="B35" s="49"/>
-      <c r="C35" s="49"/>
-      <c r="D35" s="49"/>
-      <c r="E35" s="49"/>
-      <c r="F35" s="49"/>
-      <c r="G35" s="49"/>
-      <c r="H35" s="50"/>
-      <c r="I35" s="52"/>
-      <c r="J35" s="54"/>
-      <c r="K35" s="52"/>
-      <c r="L35" s="52"/>
-      <c r="M35" s="52"/>
-      <c r="N35" s="52"/>
-      <c r="O35" s="52"/>
-      <c r="P35" s="52"/>
-    </row>
-    <row r="36" spans="1:16" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="75" t="s">
-        <v>52</v>
-      </c>
-      <c r="B36" s="76"/>
-      <c r="C36" s="76"/>
-      <c r="D36" s="76"/>
-      <c r="E36" s="76"/>
-      <c r="F36" s="76"/>
-      <c r="G36" s="76"/>
-      <c r="H36" s="77"/>
-      <c r="I36" s="52"/>
-      <c r="J36" s="54"/>
-      <c r="K36" s="52"/>
-      <c r="L36" s="52"/>
-      <c r="M36" s="52"/>
-      <c r="N36" s="52"/>
-      <c r="O36" s="52"/>
-      <c r="P36" s="52"/>
+      <c r="B36" s="79"/>
+      <c r="C36" s="79"/>
+      <c r="D36" s="79"/>
+      <c r="E36" s="79"/>
+      <c r="F36" s="79"/>
+      <c r="G36" s="79"/>
+      <c r="H36" s="80"/>
+      <c r="I36" s="36"/>
+      <c r="J36" s="38"/>
+      <c r="K36" s="36"/>
+      <c r="L36" s="36"/>
+      <c r="M36" s="36"/>
+      <c r="N36" s="36"/>
+      <c r="O36" s="36"/>
+      <c r="P36" s="36"/>
     </row>
     <row r="37" spans="1:16" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="72" t="s">
+      <c r="A37" s="81" t="s">
         <v>2</v>
       </c>
-      <c r="B37" s="73"/>
-      <c r="C37" s="73"/>
-      <c r="D37" s="73"/>
-      <c r="E37" s="73"/>
-      <c r="F37" s="73"/>
-      <c r="G37" s="73"/>
-      <c r="H37" s="74"/>
+      <c r="B37" s="82"/>
+      <c r="C37" s="82"/>
+      <c r="D37" s="82"/>
+      <c r="E37" s="82"/>
+      <c r="F37" s="82"/>
+      <c r="G37" s="82"/>
+      <c r="H37" s="83"/>
     </row>
     <row r="38" spans="1:16" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="72" t="s">
+      <c r="A38" s="81" t="s">
         <v>3</v>
       </c>
-      <c r="B38" s="73"/>
-      <c r="C38" s="73"/>
-      <c r="D38" s="73"/>
-      <c r="E38" s="73"/>
-      <c r="F38" s="73"/>
-      <c r="G38" s="73"/>
-      <c r="H38" s="74"/>
+      <c r="B38" s="82"/>
+      <c r="C38" s="82"/>
+      <c r="D38" s="82"/>
+      <c r="E38" s="82"/>
+      <c r="F38" s="82"/>
+      <c r="G38" s="82"/>
+      <c r="H38" s="83"/>
     </row>
     <row r="39" spans="1:16" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A39" s="30"/>
@@ -35008,34 +34981,33 @@
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0"/>
-  <mergeCells count="52">
-    <mergeCell ref="A36:H36"/>
+  <mergeCells count="51">
     <mergeCell ref="A37:H37"/>
     <mergeCell ref="A38:H38"/>
-    <mergeCell ref="A34:H34"/>
     <mergeCell ref="A28:B28"/>
     <mergeCell ref="C28:H28"/>
     <mergeCell ref="A31:B31"/>
     <mergeCell ref="A32:B32"/>
     <mergeCell ref="A33:B33"/>
     <mergeCell ref="A35:H35"/>
-    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="C31:H31"/>
+    <mergeCell ref="C32:H32"/>
+    <mergeCell ref="C33:H33"/>
     <mergeCell ref="A26:B26"/>
     <mergeCell ref="A27:B27"/>
     <mergeCell ref="A29:B29"/>
     <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A36:H36"/>
     <mergeCell ref="A21:B21"/>
     <mergeCell ref="A22:B22"/>
     <mergeCell ref="A23:B23"/>
     <mergeCell ref="A24:B24"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="A25:B25"/>
     <mergeCell ref="A18:H18"/>
     <mergeCell ref="A19:B19"/>
     <mergeCell ref="A17:H17"/>
     <mergeCell ref="C19:H19"/>
+    <mergeCell ref="A20:B20"/>
     <mergeCell ref="C20:H20"/>
     <mergeCell ref="C21:H21"/>
     <mergeCell ref="C22:H22"/>
@@ -35046,9 +35018,6 @@
     <mergeCell ref="C27:H27"/>
     <mergeCell ref="C29:H29"/>
     <mergeCell ref="C30:H30"/>
-    <mergeCell ref="C31:H31"/>
-    <mergeCell ref="C32:H32"/>
-    <mergeCell ref="C33:H33"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A12:H12"/>
     <mergeCell ref="D5:F11"/>
@@ -35061,6 +35030,9 @@
     <mergeCell ref="A9:C9"/>
     <mergeCell ref="A10:C10"/>
     <mergeCell ref="A11:C11"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B3:H3"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.43307086614173229" right="0.43307086614173229" top="0.51181102362204722" bottom="0.51181102362204722" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -35070,24 +35042,4 @@
   </headerFooter>
   <drawing r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36911788-0043-4A57-B088-78CB6C6595FB}">
-  <dimension ref="F6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="6" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
For Emp and Customer Status and Quote Detail Changes
</commit_message>
<xml_diff>
--- a/NtierMvc/App_Data/Documents/Excel/QuotePreparation.xlsx
+++ b/NtierMvc/App_Data/Documents/Excel/QuotePreparation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Deepak\Downloads\C#\NtierMvc\App_Data\Documents\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8854AA02-2C26-4617-B815-110BC9EC12C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D2A5B2E-5BE2-4BDA-83DB-028B3DA28F94}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -280,7 +280,7 @@
     <t>Manufacturer</t>
   </si>
   <si>
-    <t xml:space="preserve">Amount in Words: </t>
+    <t>Amount in Words: #AmountInWords</t>
   </si>
 </sst>
 </file>
@@ -810,6 +810,101 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
     </xf>
@@ -865,14 +960,6 @@
       <alignment horizontal="left" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
@@ -903,93 +990,6 @@
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -1400,8 +1400,8 @@
   </sheetPr>
   <dimension ref="A1:XFD43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18:H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1421,16 +1421,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16384" s="34" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="70" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
+      <c r="H1" s="70"/>
       <c r="I1" s="35"/>
       <c r="J1" s="40"/>
       <c r="K1" s="35"/>
@@ -1441,42 +1441,42 @@
       <c r="P1" s="35"/>
     </row>
     <row r="2" spans="1:16384" s="4" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="65"/>
-      <c r="B2" s="62" t="s">
+      <c r="A2" s="87"/>
+      <c r="B2" s="84" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="63"/>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63"/>
-      <c r="F2" s="63"/>
-      <c r="G2" s="63"/>
-      <c r="H2" s="64"/>
+      <c r="C2" s="85"/>
+      <c r="D2" s="85"/>
+      <c r="E2" s="85"/>
+      <c r="F2" s="85"/>
+      <c r="G2" s="85"/>
+      <c r="H2" s="86"/>
       <c r="J2" s="41"/>
     </row>
     <row r="3" spans="1:16384" s="4" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="66"/>
-      <c r="B3" s="67" t="s">
+      <c r="A3" s="88"/>
+      <c r="B3" s="89" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="68"/>
-      <c r="D3" s="68"/>
-      <c r="E3" s="68"/>
-      <c r="F3" s="68"/>
-      <c r="G3" s="68"/>
-      <c r="H3" s="69"/>
+      <c r="C3" s="90"/>
+      <c r="D3" s="90"/>
+      <c r="E3" s="90"/>
+      <c r="F3" s="90"/>
+      <c r="G3" s="90"/>
+      <c r="H3" s="91"/>
       <c r="J3" s="38"/>
     </row>
     <row r="4" spans="1:16384" s="4" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="50" t="s">
+      <c r="A4" s="74" t="s">
         <v>42</v>
       </c>
-      <c r="B4" s="50"/>
-      <c r="C4" s="50"/>
-      <c r="D4" s="47" t="s">
+      <c r="B4" s="74"/>
+      <c r="C4" s="74"/>
+      <c r="D4" s="71" t="s">
         <v>41</v>
       </c>
-      <c r="E4" s="47"/>
-      <c r="F4" s="47"/>
+      <c r="E4" s="71"/>
+      <c r="F4" s="71"/>
       <c r="G4" s="3" t="s">
         <v>40</v>
       </c>
@@ -1493,14 +1493,14 @@
       <c r="P4" s="36"/>
     </row>
     <row r="5" spans="1:16384" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="51"/>
-      <c r="B5" s="52"/>
-      <c r="C5" s="53"/>
-      <c r="D5" s="48" t="s">
+      <c r="A5" s="75"/>
+      <c r="B5" s="76"/>
+      <c r="C5" s="77"/>
+      <c r="D5" s="72" t="s">
         <v>43</v>
       </c>
-      <c r="E5" s="49"/>
-      <c r="F5" s="49"/>
+      <c r="E5" s="73"/>
+      <c r="F5" s="73"/>
       <c r="G5" s="5" t="s">
         <v>6</v>
       </c>
@@ -1517,14 +1517,14 @@
       <c r="P5" s="36"/>
     </row>
     <row r="6" spans="1:16384" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="54" t="s">
+      <c r="A6" s="78" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="55"/>
-      <c r="C6" s="56"/>
-      <c r="D6" s="48"/>
-      <c r="E6" s="49"/>
-      <c r="F6" s="49"/>
+      <c r="B6" s="79"/>
+      <c r="C6" s="80"/>
+      <c r="D6" s="72"/>
+      <c r="E6" s="73"/>
+      <c r="F6" s="73"/>
       <c r="G6" s="5" t="s">
         <v>7</v>
       </c>
@@ -1541,14 +1541,14 @@
       <c r="P6" s="36"/>
     </row>
     <row r="7" spans="1:16384" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="54" t="s">
+      <c r="A7" s="78" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="55"/>
-      <c r="C7" s="56"/>
-      <c r="D7" s="48"/>
-      <c r="E7" s="49"/>
-      <c r="F7" s="49"/>
+      <c r="B7" s="79"/>
+      <c r="C7" s="80"/>
+      <c r="D7" s="72"/>
+      <c r="E7" s="73"/>
+      <c r="F7" s="73"/>
       <c r="G7" s="5" t="s">
         <v>17</v>
       </c>
@@ -1565,14 +1565,14 @@
       <c r="P7" s="36"/>
     </row>
     <row r="8" spans="1:16384" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="54" t="s">
+      <c r="A8" s="78" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="55"/>
-      <c r="C8" s="56"/>
-      <c r="D8" s="48"/>
-      <c r="E8" s="49"/>
-      <c r="F8" s="49"/>
+      <c r="B8" s="79"/>
+      <c r="C8" s="80"/>
+      <c r="D8" s="72"/>
+      <c r="E8" s="73"/>
+      <c r="F8" s="73"/>
       <c r="G8" s="5" t="s">
         <v>19</v>
       </c>
@@ -1589,12 +1589,12 @@
       <c r="P8" s="36"/>
     </row>
     <row r="9" spans="1:16384" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="54"/>
-      <c r="B9" s="55"/>
-      <c r="C9" s="56"/>
-      <c r="D9" s="48"/>
-      <c r="E9" s="49"/>
-      <c r="F9" s="49"/>
+      <c r="A9" s="78"/>
+      <c r="B9" s="79"/>
+      <c r="C9" s="80"/>
+      <c r="D9" s="72"/>
+      <c r="E9" s="73"/>
+      <c r="F9" s="73"/>
       <c r="G9" s="5" t="s">
         <v>5</v>
       </c>
@@ -1611,12 +1611,12 @@
       <c r="P9" s="36"/>
     </row>
     <row r="10" spans="1:16384" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="54"/>
-      <c r="B10" s="55"/>
-      <c r="C10" s="56"/>
-      <c r="D10" s="48"/>
-      <c r="E10" s="49"/>
-      <c r="F10" s="49"/>
+      <c r="A10" s="78"/>
+      <c r="B10" s="79"/>
+      <c r="C10" s="80"/>
+      <c r="D10" s="72"/>
+      <c r="E10" s="73"/>
+      <c r="F10" s="73"/>
       <c r="G10" s="5" t="s">
         <v>4</v>
       </c>
@@ -1633,12 +1633,12 @@
       <c r="P10" s="36"/>
     </row>
     <row r="11" spans="1:16384" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="57"/>
-      <c r="B11" s="58"/>
-      <c r="C11" s="59"/>
-      <c r="D11" s="48"/>
-      <c r="E11" s="49"/>
-      <c r="F11" s="49"/>
+      <c r="A11" s="81"/>
+      <c r="B11" s="82"/>
+      <c r="C11" s="83"/>
+      <c r="D11" s="72"/>
+      <c r="E11" s="73"/>
+      <c r="F11" s="73"/>
       <c r="G11" s="5" t="s">
         <v>11</v>
       </c>
@@ -1655,16 +1655,16 @@
       <c r="P11" s="36"/>
     </row>
     <row r="12" spans="1:16384" s="4" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="47" t="s">
+      <c r="A12" s="71" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="47"/>
-      <c r="C12" s="47"/>
-      <c r="D12" s="47"/>
-      <c r="E12" s="47"/>
-      <c r="F12" s="47"/>
-      <c r="G12" s="47"/>
-      <c r="H12" s="47"/>
+      <c r="B12" s="71"/>
+      <c r="C12" s="71"/>
+      <c r="D12" s="71"/>
+      <c r="E12" s="71"/>
+      <c r="F12" s="71"/>
+      <c r="G12" s="71"/>
+      <c r="H12" s="71"/>
       <c r="I12" s="36"/>
       <c r="K12" s="36"/>
       <c r="L12" s="36"/>
@@ -18076,7 +18076,7 @@
       <c r="XFD13" s="4"/>
     </row>
     <row r="14" spans="1:16384" s="13" customFormat="1" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A14" s="90"/>
+      <c r="A14" s="46"/>
       <c r="B14" s="14"/>
       <c r="C14" s="15"/>
       <c r="D14" s="16"/>
@@ -34462,7 +34462,7 @@
       <c r="XFD14" s="4"/>
     </row>
     <row r="15" spans="1:16384" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="91"/>
+      <c r="A15" s="47"/>
       <c r="B15" s="18"/>
       <c r="C15" s="19"/>
       <c r="D15" s="18"/>
@@ -34494,16 +34494,16 @@
       <c r="P16" s="38"/>
     </row>
     <row r="17" spans="1:16" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="75" t="s">
+      <c r="A17" s="66" t="s">
         <v>70</v>
       </c>
-      <c r="B17" s="76"/>
-      <c r="C17" s="76"/>
-      <c r="D17" s="76"/>
-      <c r="E17" s="76"/>
-      <c r="F17" s="76"/>
-      <c r="G17" s="76"/>
-      <c r="H17" s="77"/>
+      <c r="B17" s="67"/>
+      <c r="C17" s="67"/>
+      <c r="D17" s="67"/>
+      <c r="E17" s="67"/>
+      <c r="F17" s="67"/>
+      <c r="G17" s="67"/>
+      <c r="H17" s="68"/>
       <c r="J17" s="38"/>
       <c r="K17" s="36"/>
       <c r="L17" s="36"/>
@@ -34513,16 +34513,16 @@
       <c r="P17" s="36"/>
     </row>
     <row r="18" spans="1:16" s="2" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="70" t="s">
+      <c r="A18" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="B18" s="71"/>
-      <c r="C18" s="71"/>
-      <c r="D18" s="71"/>
-      <c r="E18" s="71"/>
-      <c r="F18" s="71"/>
-      <c r="G18" s="71"/>
-      <c r="H18" s="72"/>
+      <c r="B18" s="64"/>
+      <c r="C18" s="64"/>
+      <c r="D18" s="64"/>
+      <c r="E18" s="64"/>
+      <c r="F18" s="64"/>
+      <c r="G18" s="64"/>
+      <c r="H18" s="65"/>
       <c r="I18" s="36"/>
       <c r="J18" s="38"/>
       <c r="K18" s="36"/>
@@ -34533,18 +34533,18 @@
       <c r="P18" s="36"/>
     </row>
     <row r="19" spans="1:16" s="2" customFormat="1" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="73" t="s">
+      <c r="A19" s="51" t="s">
         <v>57</v>
       </c>
-      <c r="B19" s="74"/>
-      <c r="C19" s="61" t="s">
+      <c r="B19" s="52"/>
+      <c r="C19" s="69" t="s">
         <v>36</v>
       </c>
-      <c r="D19" s="61"/>
-      <c r="E19" s="61"/>
-      <c r="F19" s="61"/>
-      <c r="G19" s="61"/>
-      <c r="H19" s="61"/>
+      <c r="D19" s="69"/>
+      <c r="E19" s="69"/>
+      <c r="F19" s="69"/>
+      <c r="G19" s="69"/>
+      <c r="H19" s="69"/>
       <c r="I19" s="36"/>
       <c r="J19" s="38"/>
       <c r="K19" s="36"/>
@@ -34555,16 +34555,16 @@
       <c r="P19" s="36"/>
     </row>
     <row r="20" spans="1:16" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="73" t="s">
+      <c r="A20" s="51" t="s">
         <v>58</v>
       </c>
-      <c r="B20" s="74"/>
-      <c r="C20" s="60"/>
-      <c r="D20" s="60"/>
-      <c r="E20" s="60"/>
-      <c r="F20" s="60"/>
-      <c r="G20" s="60"/>
-      <c r="H20" s="60"/>
+      <c r="B20" s="52"/>
+      <c r="C20" s="59"/>
+      <c r="D20" s="59"/>
+      <c r="E20" s="59"/>
+      <c r="F20" s="59"/>
+      <c r="G20" s="59"/>
+      <c r="H20" s="59"/>
       <c r="I20" s="36"/>
       <c r="J20" s="38"/>
       <c r="K20" s="36"/>
@@ -34575,18 +34575,18 @@
       <c r="P20" s="36"/>
     </row>
     <row r="21" spans="1:16" s="2" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="73" t="s">
+      <c r="A21" s="51" t="s">
         <v>59</v>
       </c>
-      <c r="B21" s="74"/>
-      <c r="C21" s="60" t="s">
+      <c r="B21" s="52"/>
+      <c r="C21" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="D21" s="60"/>
-      <c r="E21" s="60"/>
-      <c r="F21" s="60"/>
-      <c r="G21" s="60"/>
-      <c r="H21" s="60"/>
+      <c r="D21" s="59"/>
+      <c r="E21" s="59"/>
+      <c r="F21" s="59"/>
+      <c r="G21" s="59"/>
+      <c r="H21" s="59"/>
       <c r="I21" s="36"/>
       <c r="J21" s="38"/>
       <c r="K21" s="36"/>
@@ -34597,18 +34597,18 @@
       <c r="P21" s="36"/>
     </row>
     <row r="22" spans="1:16" s="2" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="73" t="s">
+      <c r="A22" s="51" t="s">
         <v>60</v>
       </c>
-      <c r="B22" s="74"/>
-      <c r="C22" s="60" t="s">
+      <c r="B22" s="52"/>
+      <c r="C22" s="59" t="s">
         <v>30</v>
       </c>
-      <c r="D22" s="60"/>
-      <c r="E22" s="60"/>
-      <c r="F22" s="60"/>
-      <c r="G22" s="60"/>
-      <c r="H22" s="60"/>
+      <c r="D22" s="59"/>
+      <c r="E22" s="59"/>
+      <c r="F22" s="59"/>
+      <c r="G22" s="59"/>
+      <c r="H22" s="59"/>
       <c r="I22" s="36"/>
       <c r="J22" s="38"/>
       <c r="K22" s="36"/>
@@ -34619,18 +34619,18 @@
       <c r="P22" s="36"/>
     </row>
     <row r="23" spans="1:16" s="2" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="73" t="s">
+      <c r="A23" s="51" t="s">
         <v>61</v>
       </c>
-      <c r="B23" s="74"/>
-      <c r="C23" s="61" t="s">
+      <c r="B23" s="52"/>
+      <c r="C23" s="69" t="s">
         <v>51</v>
       </c>
-      <c r="D23" s="61"/>
-      <c r="E23" s="61"/>
-      <c r="F23" s="61"/>
-      <c r="G23" s="61"/>
-      <c r="H23" s="61"/>
+      <c r="D23" s="69"/>
+      <c r="E23" s="69"/>
+      <c r="F23" s="69"/>
+      <c r="G23" s="69"/>
+      <c r="H23" s="69"/>
       <c r="I23" s="36"/>
       <c r="J23" s="38"/>
       <c r="K23" s="36"/>
@@ -34641,18 +34641,18 @@
       <c r="P23" s="36"/>
     </row>
     <row r="24" spans="1:16" s="2" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="73" t="s">
+      <c r="A24" s="51" t="s">
         <v>62</v>
       </c>
-      <c r="B24" s="74"/>
-      <c r="C24" s="60" t="s">
+      <c r="B24" s="52"/>
+      <c r="C24" s="59" t="s">
         <v>12</v>
       </c>
-      <c r="D24" s="60"/>
-      <c r="E24" s="60"/>
-      <c r="F24" s="60"/>
-      <c r="G24" s="60"/>
-      <c r="H24" s="60"/>
+      <c r="D24" s="59"/>
+      <c r="E24" s="59"/>
+      <c r="F24" s="59"/>
+      <c r="G24" s="59"/>
+      <c r="H24" s="59"/>
       <c r="I24" s="36"/>
       <c r="J24" s="38"/>
       <c r="K24" s="36"/>
@@ -34663,18 +34663,18 @@
       <c r="P24" s="36"/>
     </row>
     <row r="25" spans="1:16" s="2" customFormat="1" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A25" s="73" t="s">
+      <c r="A25" s="51" t="s">
         <v>63</v>
       </c>
-      <c r="B25" s="74"/>
-      <c r="C25" s="60" t="s">
+      <c r="B25" s="52"/>
+      <c r="C25" s="59" t="s">
         <v>34</v>
       </c>
-      <c r="D25" s="60"/>
-      <c r="E25" s="60"/>
-      <c r="F25" s="60"/>
-      <c r="G25" s="60"/>
-      <c r="H25" s="60"/>
+      <c r="D25" s="59"/>
+      <c r="E25" s="59"/>
+      <c r="F25" s="59"/>
+      <c r="G25" s="59"/>
+      <c r="H25" s="59"/>
       <c r="I25" s="36"/>
       <c r="J25" s="38"/>
       <c r="K25" s="36"/>
@@ -34685,18 +34685,18 @@
       <c r="P25" s="36"/>
     </row>
     <row r="26" spans="1:16" s="2" customFormat="1" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A26" s="73" t="s">
+      <c r="A26" s="51" t="s">
         <v>64</v>
       </c>
-      <c r="B26" s="74"/>
-      <c r="C26" s="61" t="s">
+      <c r="B26" s="52"/>
+      <c r="C26" s="69" t="s">
         <v>13</v>
       </c>
-      <c r="D26" s="61"/>
-      <c r="E26" s="61"/>
-      <c r="F26" s="61"/>
-      <c r="G26" s="61"/>
-      <c r="H26" s="61"/>
+      <c r="D26" s="69"/>
+      <c r="E26" s="69"/>
+      <c r="F26" s="69"/>
+      <c r="G26" s="69"/>
+      <c r="H26" s="69"/>
       <c r="I26" s="36"/>
       <c r="J26" s="38"/>
       <c r="K26" s="36"/>
@@ -34707,18 +34707,18 @@
       <c r="P26" s="36"/>
     </row>
     <row r="27" spans="1:16" s="2" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="73" t="s">
+      <c r="A27" s="51" t="s">
         <v>65</v>
       </c>
-      <c r="B27" s="74"/>
-      <c r="C27" s="60" t="s">
+      <c r="B27" s="52"/>
+      <c r="C27" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="D27" s="60"/>
-      <c r="E27" s="60"/>
-      <c r="F27" s="60"/>
-      <c r="G27" s="60"/>
-      <c r="H27" s="60"/>
+      <c r="D27" s="59"/>
+      <c r="E27" s="59"/>
+      <c r="F27" s="59"/>
+      <c r="G27" s="59"/>
+      <c r="H27" s="59"/>
       <c r="I27" s="36"/>
       <c r="J27" s="38"/>
       <c r="K27" s="36"/>
@@ -34729,18 +34729,18 @@
       <c r="P27" s="36"/>
     </row>
     <row r="28" spans="1:16" s="2" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="73" t="s">
+      <c r="A28" s="51" t="s">
         <v>52</v>
       </c>
-      <c r="B28" s="74"/>
-      <c r="C28" s="84" t="s">
+      <c r="B28" s="52"/>
+      <c r="C28" s="53" t="s">
         <v>53</v>
       </c>
-      <c r="D28" s="85"/>
-      <c r="E28" s="85"/>
-      <c r="F28" s="85"/>
-      <c r="G28" s="85"/>
-      <c r="H28" s="86"/>
+      <c r="D28" s="54"/>
+      <c r="E28" s="54"/>
+      <c r="F28" s="54"/>
+      <c r="G28" s="54"/>
+      <c r="H28" s="55"/>
       <c r="J28" s="38"/>
       <c r="K28" s="36"/>
       <c r="L28" s="36"/>
@@ -34750,18 +34750,18 @@
       <c r="P28" s="36"/>
     </row>
     <row r="29" spans="1:16" s="2" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="73" t="s">
+      <c r="A29" s="51" t="s">
         <v>66</v>
       </c>
-      <c r="B29" s="74"/>
-      <c r="C29" s="61" t="s">
+      <c r="B29" s="52"/>
+      <c r="C29" s="69" t="s">
         <v>15</v>
       </c>
-      <c r="D29" s="61"/>
-      <c r="E29" s="61"/>
-      <c r="F29" s="61"/>
-      <c r="G29" s="61"/>
-      <c r="H29" s="61"/>
+      <c r="D29" s="69"/>
+      <c r="E29" s="69"/>
+      <c r="F29" s="69"/>
+      <c r="G29" s="69"/>
+      <c r="H29" s="69"/>
       <c r="I29" s="36"/>
       <c r="K29" s="36"/>
       <c r="L29" s="36"/>
@@ -34771,18 +34771,18 @@
       <c r="P29" s="36"/>
     </row>
     <row r="30" spans="1:16" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="73" t="s">
+      <c r="A30" s="51" t="s">
         <v>67</v>
       </c>
-      <c r="B30" s="74"/>
-      <c r="C30" s="60" t="s">
+      <c r="B30" s="52"/>
+      <c r="C30" s="59" t="s">
         <v>54</v>
       </c>
-      <c r="D30" s="60"/>
-      <c r="E30" s="60"/>
-      <c r="F30" s="60"/>
-      <c r="G30" s="60"/>
-      <c r="H30" s="60"/>
+      <c r="D30" s="59"/>
+      <c r="E30" s="59"/>
+      <c r="F30" s="59"/>
+      <c r="G30" s="59"/>
+      <c r="H30" s="59"/>
       <c r="I30" s="36"/>
       <c r="J30" s="38"/>
       <c r="K30" s="36"/>
@@ -34793,18 +34793,18 @@
       <c r="P30" s="36"/>
     </row>
     <row r="31" spans="1:16" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="73" t="s">
+      <c r="A31" s="51" t="s">
         <v>68</v>
       </c>
-      <c r="B31" s="74"/>
-      <c r="C31" s="60" t="s">
+      <c r="B31" s="52"/>
+      <c r="C31" s="59" t="s">
         <v>16</v>
       </c>
-      <c r="D31" s="60"/>
-      <c r="E31" s="60"/>
-      <c r="F31" s="60"/>
-      <c r="G31" s="60"/>
-      <c r="H31" s="60"/>
+      <c r="D31" s="59"/>
+      <c r="E31" s="59"/>
+      <c r="F31" s="59"/>
+      <c r="G31" s="59"/>
+      <c r="H31" s="59"/>
       <c r="I31" s="36"/>
       <c r="J31" s="38"/>
       <c r="K31" s="36"/>
@@ -34815,18 +34815,18 @@
       <c r="P31" s="36"/>
     </row>
     <row r="32" spans="1:16" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="73" t="s">
+      <c r="A32" s="51" t="s">
         <v>56</v>
       </c>
-      <c r="B32" s="74"/>
-      <c r="C32" s="60" t="s">
+      <c r="B32" s="52"/>
+      <c r="C32" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="D32" s="60"/>
-      <c r="E32" s="60"/>
-      <c r="F32" s="60"/>
-      <c r="G32" s="60"/>
-      <c r="H32" s="60"/>
+      <c r="D32" s="59"/>
+      <c r="E32" s="59"/>
+      <c r="F32" s="59"/>
+      <c r="G32" s="59"/>
+      <c r="H32" s="59"/>
       <c r="I32" s="36"/>
       <c r="J32" s="38"/>
       <c r="K32" s="36"/>
@@ -34837,18 +34837,18 @@
       <c r="P32" s="36"/>
     </row>
     <row r="33" spans="1:16" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="73" t="s">
+      <c r="A33" s="51" t="s">
         <v>69</v>
       </c>
-      <c r="B33" s="74"/>
-      <c r="C33" s="60" t="s">
+      <c r="B33" s="52"/>
+      <c r="C33" s="59" t="s">
         <v>55</v>
       </c>
-      <c r="D33" s="60"/>
-      <c r="E33" s="60"/>
-      <c r="F33" s="60"/>
-      <c r="G33" s="60"/>
-      <c r="H33" s="60"/>
+      <c r="D33" s="59"/>
+      <c r="E33" s="59"/>
+      <c r="F33" s="59"/>
+      <c r="G33" s="59"/>
+      <c r="H33" s="59"/>
       <c r="I33" s="36"/>
       <c r="J33" s="38"/>
       <c r="K33" s="36"/>
@@ -34879,16 +34879,16 @@
       <c r="P34" s="36"/>
     </row>
     <row r="35" spans="1:16" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="87" t="s">
+      <c r="A35" s="56" t="s">
         <v>49</v>
       </c>
-      <c r="B35" s="88"/>
-      <c r="C35" s="88"/>
-      <c r="D35" s="88"/>
-      <c r="E35" s="88"/>
-      <c r="F35" s="88"/>
-      <c r="G35" s="88"/>
-      <c r="H35" s="89"/>
+      <c r="B35" s="57"/>
+      <c r="C35" s="57"/>
+      <c r="D35" s="57"/>
+      <c r="E35" s="57"/>
+      <c r="F35" s="57"/>
+      <c r="G35" s="57"/>
+      <c r="H35" s="58"/>
       <c r="I35" s="36"/>
       <c r="J35" s="38"/>
       <c r="K35" s="36"/>
@@ -34899,16 +34899,16 @@
       <c r="P35" s="36"/>
     </row>
     <row r="36" spans="1:16" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="78" t="s">
+      <c r="A36" s="60" t="s">
         <v>50</v>
       </c>
-      <c r="B36" s="79"/>
-      <c r="C36" s="79"/>
-      <c r="D36" s="79"/>
-      <c r="E36" s="79"/>
-      <c r="F36" s="79"/>
-      <c r="G36" s="79"/>
-      <c r="H36" s="80"/>
+      <c r="B36" s="61"/>
+      <c r="C36" s="61"/>
+      <c r="D36" s="61"/>
+      <c r="E36" s="61"/>
+      <c r="F36" s="61"/>
+      <c r="G36" s="61"/>
+      <c r="H36" s="62"/>
       <c r="I36" s="36"/>
       <c r="J36" s="38"/>
       <c r="K36" s="36"/>
@@ -34919,28 +34919,28 @@
       <c r="P36" s="36"/>
     </row>
     <row r="37" spans="1:16" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="81" t="s">
+      <c r="A37" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="B37" s="82"/>
-      <c r="C37" s="82"/>
-      <c r="D37" s="82"/>
-      <c r="E37" s="82"/>
-      <c r="F37" s="82"/>
-      <c r="G37" s="82"/>
-      <c r="H37" s="83"/>
+      <c r="B37" s="49"/>
+      <c r="C37" s="49"/>
+      <c r="D37" s="49"/>
+      <c r="E37" s="49"/>
+      <c r="F37" s="49"/>
+      <c r="G37" s="49"/>
+      <c r="H37" s="50"/>
     </row>
     <row r="38" spans="1:16" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="81" t="s">
+      <c r="A38" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="B38" s="82"/>
-      <c r="C38" s="82"/>
-      <c r="D38" s="82"/>
-      <c r="E38" s="82"/>
-      <c r="F38" s="82"/>
-      <c r="G38" s="82"/>
-      <c r="H38" s="83"/>
+      <c r="B38" s="49"/>
+      <c r="C38" s="49"/>
+      <c r="D38" s="49"/>
+      <c r="E38" s="49"/>
+      <c r="F38" s="49"/>
+      <c r="G38" s="49"/>
+      <c r="H38" s="50"/>
     </row>
     <row r="39" spans="1:16" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A39" s="30"/>
@@ -34982,42 +34982,6 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="51">
-    <mergeCell ref="A37:H37"/>
-    <mergeCell ref="A38:H38"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="C28:H28"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A35:H35"/>
-    <mergeCell ref="C31:H31"/>
-    <mergeCell ref="C32:H32"/>
-    <mergeCell ref="C33:H33"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A36:H36"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A18:H18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A17:H17"/>
-    <mergeCell ref="C19:H19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="C20:H20"/>
-    <mergeCell ref="C21:H21"/>
-    <mergeCell ref="C22:H22"/>
-    <mergeCell ref="C23:H23"/>
-    <mergeCell ref="C24:H24"/>
-    <mergeCell ref="C25:H25"/>
-    <mergeCell ref="C26:H26"/>
-    <mergeCell ref="C27:H27"/>
-    <mergeCell ref="C29:H29"/>
-    <mergeCell ref="C30:H30"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A12:H12"/>
     <mergeCell ref="D5:F11"/>
@@ -35033,6 +34997,42 @@
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B3:H3"/>
+    <mergeCell ref="C21:H21"/>
+    <mergeCell ref="C22:H22"/>
+    <mergeCell ref="C23:H23"/>
+    <mergeCell ref="C24:H24"/>
+    <mergeCell ref="C25:H25"/>
+    <mergeCell ref="A18:H18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A17:H17"/>
+    <mergeCell ref="C19:H19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="C20:H20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A36:H36"/>
+    <mergeCell ref="C26:H26"/>
+    <mergeCell ref="C27:H27"/>
+    <mergeCell ref="C29:H29"/>
+    <mergeCell ref="C30:H30"/>
+    <mergeCell ref="A37:H37"/>
+    <mergeCell ref="A38:H38"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="C28:H28"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A35:H35"/>
+    <mergeCell ref="C31:H31"/>
+    <mergeCell ref="C32:H32"/>
+    <mergeCell ref="C33:H33"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.43307086614173229" right="0.43307086614173229" top="0.51181102362204722" bottom="0.51181102362204722" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>

<commit_message>
For Mackarel Changes By Daniel 27-02-2021
</commit_message>
<xml_diff>
--- a/NtierMvc/App_Data/Documents/Excel/QuotePreparation.xlsx
+++ b/NtierMvc/App_Data/Documents/Excel/QuotePreparation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Deepak\Downloads\C#\NtierMvc\App_Data\Documents\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{643219A6-91D6-4CCC-9A30-92E6F53D6CDA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4579F077-95CF-4CC4-A3A4-6E293ADA38B9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="11070" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -638,7 +638,7 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
@@ -701,10 +701,6 @@
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -785,10 +781,6 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -805,7 +797,92 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -893,94 +970,6 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -1391,8 +1380,8 @@
   </sheetPr>
   <dimension ref="A1:P43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1405,266 +1394,266 @@
     <col min="6" max="6" width="19.28515625" style="1" customWidth="1"/>
     <col min="7" max="7" width="25.42578125" style="1" customWidth="1"/>
     <col min="8" max="8" width="26.85546875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="32"/>
-    <col min="10" max="10" width="9.140625" style="37"/>
-    <col min="11" max="16" width="9.140625" style="32"/>
+    <col min="9" max="9" width="9.140625" style="31"/>
+    <col min="10" max="10" width="9.140625" style="36"/>
+    <col min="11" max="16" width="9.140625" style="31"/>
     <col min="17" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="47" t="s">
+    <row r="1" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="66" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="30"/>
-      <c r="N1" s="30"/>
-      <c r="O1" s="30"/>
-      <c r="P1" s="30"/>
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
+      <c r="H1" s="66"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29"/>
+      <c r="O1" s="29"/>
+      <c r="P1" s="29"/>
     </row>
     <row r="2" spans="1:16" s="4" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="64"/>
-      <c r="B2" s="61" t="s">
+      <c r="A2" s="83"/>
+      <c r="B2" s="80" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62"/>
-      <c r="F2" s="62"/>
-      <c r="G2" s="62"/>
-      <c r="H2" s="63"/>
-      <c r="J2" s="36"/>
+      <c r="C2" s="81"/>
+      <c r="D2" s="81"/>
+      <c r="E2" s="81"/>
+      <c r="F2" s="81"/>
+      <c r="G2" s="81"/>
+      <c r="H2" s="82"/>
+      <c r="J2" s="35"/>
     </row>
     <row r="3" spans="1:16" s="4" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="65"/>
-      <c r="B3" s="66" t="s">
+      <c r="A3" s="84"/>
+      <c r="B3" s="85" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="67"/>
-      <c r="D3" s="67"/>
-      <c r="E3" s="67"/>
-      <c r="F3" s="67"/>
-      <c r="G3" s="67"/>
-      <c r="H3" s="68"/>
-      <c r="J3" s="33"/>
+      <c r="C3" s="86"/>
+      <c r="D3" s="86"/>
+      <c r="E3" s="86"/>
+      <c r="F3" s="86"/>
+      <c r="G3" s="86"/>
+      <c r="H3" s="87"/>
+      <c r="J3" s="32"/>
     </row>
     <row r="4" spans="1:16" s="4" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="51" t="s">
+      <c r="A4" s="70" t="s">
         <v>40</v>
       </c>
-      <c r="B4" s="51"/>
-      <c r="C4" s="51"/>
-      <c r="D4" s="48" t="s">
+      <c r="B4" s="70"/>
+      <c r="C4" s="70"/>
+      <c r="D4" s="67" t="s">
         <v>39</v>
       </c>
-      <c r="E4" s="48"/>
-      <c r="F4" s="48"/>
+      <c r="E4" s="67"/>
+      <c r="F4" s="67"/>
       <c r="G4" s="3" t="s">
         <v>38</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="I4" s="31"/>
-      <c r="J4" s="33"/>
-      <c r="K4" s="31"/>
-      <c r="L4" s="31"/>
-      <c r="M4" s="31"/>
-      <c r="N4" s="31"/>
-      <c r="O4" s="31"/>
-      <c r="P4" s="31"/>
+      <c r="I4" s="30"/>
+      <c r="J4" s="32"/>
+      <c r="K4" s="30"/>
+      <c r="L4" s="30"/>
+      <c r="M4" s="30"/>
+      <c r="N4" s="30"/>
+      <c r="O4" s="30"/>
+      <c r="P4" s="30"/>
     </row>
     <row r="5" spans="1:16" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="52"/>
-      <c r="B5" s="53"/>
-      <c r="C5" s="54"/>
-      <c r="D5" s="49" t="s">
+      <c r="A5" s="71"/>
+      <c r="B5" s="72"/>
+      <c r="C5" s="73"/>
+      <c r="D5" s="68" t="s">
         <v>41</v>
       </c>
-      <c r="E5" s="50"/>
-      <c r="F5" s="50"/>
+      <c r="E5" s="69"/>
+      <c r="F5" s="69"/>
       <c r="G5" s="5" t="s">
         <v>6</v>
       </c>
       <c r="H5" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="I5" s="31"/>
-      <c r="J5" s="33"/>
-      <c r="K5" s="31"/>
-      <c r="L5" s="31"/>
-      <c r="M5" s="31"/>
-      <c r="N5" s="31"/>
-      <c r="O5" s="31"/>
-      <c r="P5" s="31"/>
+      <c r="I5" s="30"/>
+      <c r="J5" s="32"/>
+      <c r="K5" s="30"/>
+      <c r="L5" s="30"/>
+      <c r="M5" s="30"/>
+      <c r="N5" s="30"/>
+      <c r="O5" s="30"/>
+      <c r="P5" s="30"/>
     </row>
     <row r="6" spans="1:16" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="55" t="s">
+      <c r="A6" s="74" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="56"/>
-      <c r="C6" s="57"/>
-      <c r="D6" s="49"/>
-      <c r="E6" s="50"/>
-      <c r="F6" s="50"/>
+      <c r="B6" s="75"/>
+      <c r="C6" s="76"/>
+      <c r="D6" s="68"/>
+      <c r="E6" s="69"/>
+      <c r="F6" s="69"/>
       <c r="G6" s="5" t="s">
         <v>7</v>
       </c>
       <c r="H6" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="I6" s="31"/>
-      <c r="J6" s="33"/>
-      <c r="K6" s="31"/>
-      <c r="L6" s="31"/>
-      <c r="M6" s="31"/>
-      <c r="N6" s="31"/>
-      <c r="O6" s="31"/>
-      <c r="P6" s="31"/>
+      <c r="I6" s="30"/>
+      <c r="J6" s="32"/>
+      <c r="K6" s="30"/>
+      <c r="L6" s="30"/>
+      <c r="M6" s="30"/>
+      <c r="N6" s="30"/>
+      <c r="O6" s="30"/>
+      <c r="P6" s="30"/>
     </row>
     <row r="7" spans="1:16" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="55" t="s">
+      <c r="A7" s="74" t="s">
         <v>71</v>
       </c>
-      <c r="B7" s="56"/>
-      <c r="C7" s="57"/>
-      <c r="D7" s="49"/>
-      <c r="E7" s="50"/>
-      <c r="F7" s="50"/>
+      <c r="B7" s="75"/>
+      <c r="C7" s="76"/>
+      <c r="D7" s="68"/>
+      <c r="E7" s="69"/>
+      <c r="F7" s="69"/>
       <c r="G7" s="5" t="s">
         <v>17</v>
       </c>
       <c r="H7" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="I7" s="31"/>
-      <c r="J7" s="33"/>
-      <c r="K7" s="31"/>
-      <c r="L7" s="31"/>
-      <c r="M7" s="31"/>
-      <c r="N7" s="31"/>
-      <c r="O7" s="31"/>
-      <c r="P7" s="31"/>
+      <c r="I7" s="30"/>
+      <c r="J7" s="32"/>
+      <c r="K7" s="30"/>
+      <c r="L7" s="30"/>
+      <c r="M7" s="30"/>
+      <c r="N7" s="30"/>
+      <c r="O7" s="30"/>
+      <c r="P7" s="30"/>
     </row>
     <row r="8" spans="1:16" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="55" t="s">
+      <c r="A8" s="74" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="56"/>
-      <c r="C8" s="57"/>
-      <c r="D8" s="49"/>
-      <c r="E8" s="50"/>
-      <c r="F8" s="50"/>
+      <c r="B8" s="75"/>
+      <c r="C8" s="76"/>
+      <c r="D8" s="68"/>
+      <c r="E8" s="69"/>
+      <c r="F8" s="69"/>
       <c r="G8" s="5" t="s">
         <v>19</v>
       </c>
       <c r="H8" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="I8" s="31"/>
-      <c r="J8" s="33"/>
-      <c r="K8" s="31"/>
-      <c r="L8" s="31"/>
-      <c r="M8" s="31"/>
-      <c r="N8" s="31"/>
-      <c r="O8" s="31"/>
-      <c r="P8" s="31"/>
+      <c r="I8" s="30"/>
+      <c r="J8" s="32"/>
+      <c r="K8" s="30"/>
+      <c r="L8" s="30"/>
+      <c r="M8" s="30"/>
+      <c r="N8" s="30"/>
+      <c r="O8" s="30"/>
+      <c r="P8" s="30"/>
     </row>
     <row r="9" spans="1:16" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="55" t="s">
+      <c r="A9" s="74" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="56"/>
-      <c r="C9" s="57"/>
-      <c r="D9" s="49"/>
-      <c r="E9" s="50"/>
-      <c r="F9" s="50"/>
+      <c r="B9" s="75"/>
+      <c r="C9" s="76"/>
+      <c r="D9" s="68"/>
+      <c r="E9" s="69"/>
+      <c r="F9" s="69"/>
       <c r="G9" s="5" t="s">
         <v>5</v>
       </c>
       <c r="H9" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="I9" s="31"/>
-      <c r="J9" s="33"/>
-      <c r="K9" s="31"/>
-      <c r="L9" s="31"/>
-      <c r="M9" s="31"/>
-      <c r="N9" s="31"/>
-      <c r="O9" s="31"/>
-      <c r="P9" s="31"/>
+      <c r="I9" s="30"/>
+      <c r="J9" s="32"/>
+      <c r="K9" s="30"/>
+      <c r="L9" s="30"/>
+      <c r="M9" s="30"/>
+      <c r="N9" s="30"/>
+      <c r="O9" s="30"/>
+      <c r="P9" s="30"/>
     </row>
     <row r="10" spans="1:16" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="55"/>
-      <c r="B10" s="56"/>
-      <c r="C10" s="57"/>
-      <c r="D10" s="49"/>
-      <c r="E10" s="50"/>
-      <c r="F10" s="50"/>
+      <c r="A10" s="74"/>
+      <c r="B10" s="75"/>
+      <c r="C10" s="76"/>
+      <c r="D10" s="68"/>
+      <c r="E10" s="69"/>
+      <c r="F10" s="69"/>
       <c r="G10" s="5" t="s">
         <v>4</v>
       </c>
       <c r="H10" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="I10" s="31"/>
-      <c r="J10" s="34"/>
-      <c r="K10" s="31"/>
-      <c r="L10" s="31"/>
-      <c r="M10" s="31"/>
-      <c r="N10" s="31"/>
-      <c r="O10" s="31"/>
-      <c r="P10" s="31"/>
+      <c r="I10" s="30"/>
+      <c r="J10" s="33"/>
+      <c r="K10" s="30"/>
+      <c r="L10" s="30"/>
+      <c r="M10" s="30"/>
+      <c r="N10" s="30"/>
+      <c r="O10" s="30"/>
+      <c r="P10" s="30"/>
     </row>
     <row r="11" spans="1:16" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="58"/>
-      <c r="B11" s="59"/>
-      <c r="C11" s="60"/>
-      <c r="D11" s="49"/>
-      <c r="E11" s="50"/>
-      <c r="F11" s="50"/>
+      <c r="A11" s="77"/>
+      <c r="B11" s="78"/>
+      <c r="C11" s="79"/>
+      <c r="D11" s="68"/>
+      <c r="E11" s="69"/>
+      <c r="F11" s="69"/>
       <c r="G11" s="5" t="s">
         <v>11</v>
       </c>
       <c r="H11" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="I11" s="31"/>
-      <c r="J11" s="36"/>
-      <c r="K11" s="31"/>
-      <c r="L11" s="31"/>
-      <c r="M11" s="31"/>
-      <c r="N11" s="31"/>
-      <c r="O11" s="31"/>
-      <c r="P11" s="31"/>
+      <c r="I11" s="30"/>
+      <c r="J11" s="35"/>
+      <c r="K11" s="30"/>
+      <c r="L11" s="30"/>
+      <c r="M11" s="30"/>
+      <c r="N11" s="30"/>
+      <c r="O11" s="30"/>
+      <c r="P11" s="30"/>
     </row>
     <row r="12" spans="1:16" s="4" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="48" t="s">
+      <c r="A12" s="67" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="48"/>
-      <c r="C12" s="48"/>
-      <c r="D12" s="48"/>
-      <c r="E12" s="48"/>
-      <c r="F12" s="48"/>
-      <c r="G12" s="48"/>
-      <c r="H12" s="48"/>
-      <c r="I12" s="31"/>
-      <c r="K12" s="31"/>
-      <c r="L12" s="31"/>
-      <c r="M12" s="31"/>
-      <c r="N12" s="31"/>
-      <c r="O12" s="31"/>
-      <c r="P12" s="31"/>
+      <c r="B12" s="67"/>
+      <c r="C12" s="67"/>
+      <c r="D12" s="67"/>
+      <c r="E12" s="67"/>
+      <c r="F12" s="67"/>
+      <c r="G12" s="67"/>
+      <c r="H12" s="67"/>
+      <c r="I12" s="30"/>
+      <c r="K12" s="30"/>
+      <c r="L12" s="30"/>
+      <c r="M12" s="30"/>
+      <c r="N12" s="30"/>
+      <c r="O12" s="30"/>
+      <c r="P12" s="30"/>
     </row>
     <row r="13" spans="1:16" s="4" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
@@ -1691,17 +1680,17 @@
       <c r="H13" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="I13" s="31"/>
-      <c r="J13" s="33"/>
-      <c r="K13" s="31"/>
-      <c r="L13" s="31"/>
-      <c r="M13" s="31"/>
-      <c r="N13" s="31"/>
-      <c r="O13" s="31"/>
-      <c r="P13" s="31"/>
+      <c r="I13" s="30"/>
+      <c r="J13" s="32"/>
+      <c r="K13" s="30"/>
+      <c r="L13" s="30"/>
+      <c r="M13" s="30"/>
+      <c r="N13" s="30"/>
+      <c r="O13" s="30"/>
+      <c r="P13" s="30"/>
     </row>
     <row r="14" spans="1:16" s="4" customFormat="1" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A14" s="41"/>
+      <c r="A14" s="13"/>
       <c r="B14" s="13"/>
       <c r="C14" s="14"/>
       <c r="D14" s="15"/>
@@ -1709,574 +1698,538 @@
       <c r="F14" s="16"/>
       <c r="G14" s="16"/>
       <c r="H14" s="13"/>
-      <c r="I14" s="31"/>
-      <c r="J14" s="33"/>
-      <c r="K14" s="31"/>
-      <c r="L14" s="31"/>
-      <c r="M14" s="31"/>
-      <c r="N14" s="31"/>
-      <c r="O14" s="31"/>
-      <c r="P14" s="31"/>
+      <c r="I14" s="30"/>
+      <c r="J14" s="32"/>
+      <c r="K14" s="30"/>
+      <c r="L14" s="30"/>
+      <c r="M14" s="30"/>
+      <c r="N14" s="30"/>
+      <c r="O14" s="30"/>
+      <c r="P14" s="30"/>
     </row>
     <row r="15" spans="1:16" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A15" s="46"/>
-      <c r="B15" s="42"/>
-      <c r="C15" s="43"/>
-      <c r="D15" s="42"/>
-      <c r="E15" s="42"/>
-      <c r="F15" s="44"/>
-      <c r="G15" s="45"/>
-      <c r="H15" s="42"/>
-    </row>
-    <row r="16" spans="1:16" s="24" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="17"/>
-      <c r="B16" s="18"/>
-      <c r="C16" s="19" t="s">
+      <c r="A15" s="13"/>
+      <c r="B15" s="40"/>
+      <c r="C15" s="41"/>
+      <c r="D15" s="40"/>
+      <c r="E15" s="40"/>
+      <c r="F15" s="42"/>
+      <c r="G15" s="43"/>
+      <c r="H15" s="40"/>
+    </row>
+    <row r="16" spans="1:16" s="23" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="13"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="D16" s="20"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="22" t="s">
+      <c r="D16" s="19"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="H16" s="23"/>
-      <c r="I16" s="33"/>
-      <c r="J16" s="33"/>
-      <c r="K16" s="33"/>
-      <c r="L16" s="33"/>
-      <c r="M16" s="33"/>
-      <c r="N16" s="33"/>
-      <c r="O16" s="33"/>
-      <c r="P16" s="33"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="32"/>
+      <c r="J16" s="32"/>
+      <c r="K16" s="32"/>
+      <c r="L16" s="32"/>
+      <c r="M16" s="32"/>
+      <c r="N16" s="32"/>
+      <c r="O16" s="32"/>
+      <c r="P16" s="32"/>
     </row>
     <row r="17" spans="1:16" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="76" t="s">
+      <c r="A17" s="63" t="s">
         <v>70</v>
       </c>
-      <c r="B17" s="77"/>
-      <c r="C17" s="77"/>
-      <c r="D17" s="77"/>
-      <c r="E17" s="77"/>
-      <c r="F17" s="77"/>
-      <c r="G17" s="77"/>
-      <c r="H17" s="78"/>
-      <c r="J17" s="33"/>
-      <c r="K17" s="31"/>
-      <c r="L17" s="31"/>
-      <c r="M17" s="31"/>
-      <c r="N17" s="31"/>
-      <c r="O17" s="31"/>
-      <c r="P17" s="31"/>
+      <c r="B17" s="64"/>
+      <c r="C17" s="64"/>
+      <c r="D17" s="64"/>
+      <c r="E17" s="64"/>
+      <c r="F17" s="64"/>
+      <c r="G17" s="64"/>
+      <c r="H17" s="65"/>
+      <c r="J17" s="32"/>
+      <c r="K17" s="30"/>
+      <c r="L17" s="30"/>
+      <c r="M17" s="30"/>
+      <c r="N17" s="30"/>
+      <c r="O17" s="30"/>
+      <c r="P17" s="30"/>
     </row>
     <row r="18" spans="1:16" s="2" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="71" t="s">
+      <c r="A18" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="B18" s="72"/>
-      <c r="C18" s="72"/>
-      <c r="D18" s="72"/>
-      <c r="E18" s="72"/>
-      <c r="F18" s="72"/>
-      <c r="G18" s="72"/>
-      <c r="H18" s="73"/>
-      <c r="I18" s="31"/>
-      <c r="J18" s="33"/>
-      <c r="K18" s="31"/>
-      <c r="L18" s="31"/>
-      <c r="M18" s="31"/>
-      <c r="N18" s="31"/>
-      <c r="O18" s="31"/>
-      <c r="P18" s="31"/>
+      <c r="B18" s="61"/>
+      <c r="C18" s="61"/>
+      <c r="D18" s="61"/>
+      <c r="E18" s="61"/>
+      <c r="F18" s="61"/>
+      <c r="G18" s="61"/>
+      <c r="H18" s="62"/>
+      <c r="I18" s="30"/>
+      <c r="J18" s="32"/>
+      <c r="K18" s="30"/>
+      <c r="L18" s="30"/>
+      <c r="M18" s="30"/>
+      <c r="N18" s="30"/>
+      <c r="O18" s="30"/>
+      <c r="P18" s="30"/>
     </row>
     <row r="19" spans="1:16" s="2" customFormat="1" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="74" t="s">
+      <c r="A19" s="47" t="s">
         <v>55</v>
       </c>
-      <c r="B19" s="75"/>
-      <c r="C19" s="70" t="s">
+      <c r="B19" s="48"/>
+      <c r="C19" s="59" t="s">
         <v>69</v>
       </c>
-      <c r="D19" s="70"/>
-      <c r="E19" s="70"/>
-      <c r="F19" s="70"/>
-      <c r="G19" s="70"/>
-      <c r="H19" s="70"/>
-      <c r="I19" s="31"/>
-      <c r="J19" s="33"/>
-      <c r="K19" s="31"/>
-      <c r="L19" s="31"/>
-      <c r="M19" s="31"/>
-      <c r="N19" s="31"/>
-      <c r="O19" s="31"/>
-      <c r="P19" s="31"/>
+      <c r="D19" s="59"/>
+      <c r="E19" s="59"/>
+      <c r="F19" s="59"/>
+      <c r="G19" s="59"/>
+      <c r="H19" s="59"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="32"/>
+      <c r="K19" s="30"/>
+      <c r="L19" s="30"/>
+      <c r="M19" s="30"/>
+      <c r="N19" s="30"/>
+      <c r="O19" s="30"/>
+      <c r="P19" s="30"/>
     </row>
     <row r="20" spans="1:16" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="74" t="s">
+      <c r="A20" s="47" t="s">
         <v>56</v>
       </c>
-      <c r="B20" s="75"/>
-      <c r="C20" s="69" t="s">
+      <c r="B20" s="48"/>
+      <c r="C20" s="55" t="s">
         <v>68</v>
       </c>
-      <c r="D20" s="69"/>
-      <c r="E20" s="69"/>
-      <c r="F20" s="69"/>
-      <c r="G20" s="69"/>
-      <c r="H20" s="69"/>
-      <c r="I20" s="31"/>
-      <c r="J20" s="33"/>
-      <c r="K20" s="31"/>
-      <c r="L20" s="31"/>
-      <c r="M20" s="31"/>
-      <c r="N20" s="31"/>
-      <c r="O20" s="31"/>
-      <c r="P20" s="31"/>
+      <c r="D20" s="55"/>
+      <c r="E20" s="55"/>
+      <c r="F20" s="55"/>
+      <c r="G20" s="55"/>
+      <c r="H20" s="55"/>
+      <c r="I20" s="30"/>
+      <c r="J20" s="32"/>
+      <c r="K20" s="30"/>
+      <c r="L20" s="30"/>
+      <c r="M20" s="30"/>
+      <c r="N20" s="30"/>
+      <c r="O20" s="30"/>
+      <c r="P20" s="30"/>
     </row>
     <row r="21" spans="1:16" s="2" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="74" t="s">
+      <c r="A21" s="47" t="s">
         <v>57</v>
       </c>
-      <c r="B21" s="75"/>
-      <c r="C21" s="69" t="s">
+      <c r="B21" s="48"/>
+      <c r="C21" s="55" t="s">
         <v>34</v>
       </c>
-      <c r="D21" s="69"/>
-      <c r="E21" s="69"/>
-      <c r="F21" s="69"/>
-      <c r="G21" s="69"/>
-      <c r="H21" s="69"/>
-      <c r="I21" s="31"/>
-      <c r="J21" s="33"/>
-      <c r="K21" s="31"/>
-      <c r="L21" s="31"/>
-      <c r="M21" s="31"/>
-      <c r="N21" s="31"/>
-      <c r="O21" s="31"/>
-      <c r="P21" s="31"/>
+      <c r="D21" s="55"/>
+      <c r="E21" s="55"/>
+      <c r="F21" s="55"/>
+      <c r="G21" s="55"/>
+      <c r="H21" s="55"/>
+      <c r="I21" s="30"/>
+      <c r="J21" s="32"/>
+      <c r="K21" s="30"/>
+      <c r="L21" s="30"/>
+      <c r="M21" s="30"/>
+      <c r="N21" s="30"/>
+      <c r="O21" s="30"/>
+      <c r="P21" s="30"/>
     </row>
     <row r="22" spans="1:16" s="2" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="74" t="s">
+      <c r="A22" s="47" t="s">
         <v>58</v>
       </c>
-      <c r="B22" s="75"/>
-      <c r="C22" s="69" t="s">
+      <c r="B22" s="48"/>
+      <c r="C22" s="55" t="s">
         <v>29</v>
       </c>
-      <c r="D22" s="69"/>
-      <c r="E22" s="69"/>
-      <c r="F22" s="69"/>
-      <c r="G22" s="69"/>
-      <c r="H22" s="69"/>
-      <c r="I22" s="31"/>
-      <c r="J22" s="33"/>
-      <c r="K22" s="31"/>
-      <c r="L22" s="31"/>
-      <c r="M22" s="31"/>
-      <c r="N22" s="31"/>
-      <c r="O22" s="31"/>
-      <c r="P22" s="31"/>
+      <c r="D22" s="55"/>
+      <c r="E22" s="55"/>
+      <c r="F22" s="55"/>
+      <c r="G22" s="55"/>
+      <c r="H22" s="55"/>
+      <c r="I22" s="30"/>
+      <c r="J22" s="32"/>
+      <c r="K22" s="30"/>
+      <c r="L22" s="30"/>
+      <c r="M22" s="30"/>
+      <c r="N22" s="30"/>
+      <c r="O22" s="30"/>
+      <c r="P22" s="30"/>
     </row>
     <row r="23" spans="1:16" s="2" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="74" t="s">
+      <c r="A23" s="47" t="s">
         <v>59</v>
       </c>
-      <c r="B23" s="75"/>
-      <c r="C23" s="70" t="s">
+      <c r="B23" s="48"/>
+      <c r="C23" s="59" t="s">
         <v>49</v>
       </c>
-      <c r="D23" s="70"/>
-      <c r="E23" s="70"/>
-      <c r="F23" s="70"/>
-      <c r="G23" s="70"/>
-      <c r="H23" s="70"/>
-      <c r="I23" s="31"/>
-      <c r="J23" s="33"/>
-      <c r="K23" s="31"/>
-      <c r="L23" s="31"/>
-      <c r="M23" s="31"/>
-      <c r="N23" s="31"/>
-      <c r="O23" s="31"/>
-      <c r="P23" s="31"/>
+      <c r="D23" s="59"/>
+      <c r="E23" s="59"/>
+      <c r="F23" s="59"/>
+      <c r="G23" s="59"/>
+      <c r="H23" s="59"/>
+      <c r="I23" s="30"/>
+      <c r="J23" s="32"/>
+      <c r="K23" s="30"/>
+      <c r="L23" s="30"/>
+      <c r="M23" s="30"/>
+      <c r="N23" s="30"/>
+      <c r="O23" s="30"/>
+      <c r="P23" s="30"/>
     </row>
     <row r="24" spans="1:16" s="2" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="74" t="s">
+      <c r="A24" s="47" t="s">
         <v>60</v>
       </c>
-      <c r="B24" s="75"/>
-      <c r="C24" s="69" t="s">
+      <c r="B24" s="48"/>
+      <c r="C24" s="55" t="s">
         <v>12</v>
       </c>
-      <c r="D24" s="69"/>
-      <c r="E24" s="69"/>
-      <c r="F24" s="69"/>
-      <c r="G24" s="69"/>
-      <c r="H24" s="69"/>
-      <c r="I24" s="31"/>
-      <c r="J24" s="33"/>
-      <c r="K24" s="31"/>
-      <c r="L24" s="31"/>
-      <c r="M24" s="31"/>
-      <c r="N24" s="31"/>
-      <c r="O24" s="31"/>
-      <c r="P24" s="31"/>
+      <c r="D24" s="55"/>
+      <c r="E24" s="55"/>
+      <c r="F24" s="55"/>
+      <c r="G24" s="55"/>
+      <c r="H24" s="55"/>
+      <c r="I24" s="30"/>
+      <c r="J24" s="32"/>
+      <c r="K24" s="30"/>
+      <c r="L24" s="30"/>
+      <c r="M24" s="30"/>
+      <c r="N24" s="30"/>
+      <c r="O24" s="30"/>
+      <c r="P24" s="30"/>
     </row>
     <row r="25" spans="1:16" s="2" customFormat="1" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A25" s="74" t="s">
+      <c r="A25" s="47" t="s">
         <v>61</v>
       </c>
-      <c r="B25" s="75"/>
-      <c r="C25" s="69" t="s">
+      <c r="B25" s="48"/>
+      <c r="C25" s="55" t="s">
         <v>33</v>
       </c>
-      <c r="D25" s="69"/>
-      <c r="E25" s="69"/>
-      <c r="F25" s="69"/>
-      <c r="G25" s="69"/>
-      <c r="H25" s="69"/>
-      <c r="I25" s="31"/>
-      <c r="J25" s="33"/>
-      <c r="K25" s="31"/>
-      <c r="L25" s="31"/>
-      <c r="M25" s="31"/>
-      <c r="N25" s="31"/>
-      <c r="O25" s="31"/>
-      <c r="P25" s="31"/>
+      <c r="D25" s="55"/>
+      <c r="E25" s="55"/>
+      <c r="F25" s="55"/>
+      <c r="G25" s="55"/>
+      <c r="H25" s="55"/>
+      <c r="I25" s="30"/>
+      <c r="J25" s="32"/>
+      <c r="K25" s="30"/>
+      <c r="L25" s="30"/>
+      <c r="M25" s="30"/>
+      <c r="N25" s="30"/>
+      <c r="O25" s="30"/>
+      <c r="P25" s="30"/>
     </row>
     <row r="26" spans="1:16" s="2" customFormat="1" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A26" s="74" t="s">
+      <c r="A26" s="47" t="s">
         <v>62</v>
       </c>
-      <c r="B26" s="75"/>
-      <c r="C26" s="70" t="s">
+      <c r="B26" s="48"/>
+      <c r="C26" s="59" t="s">
         <v>13</v>
       </c>
-      <c r="D26" s="70"/>
-      <c r="E26" s="70"/>
-      <c r="F26" s="70"/>
-      <c r="G26" s="70"/>
-      <c r="H26" s="70"/>
-      <c r="I26" s="31"/>
-      <c r="J26" s="33"/>
-      <c r="K26" s="31"/>
-      <c r="L26" s="31"/>
-      <c r="M26" s="31"/>
-      <c r="N26" s="31"/>
-      <c r="O26" s="31"/>
-      <c r="P26" s="31"/>
+      <c r="D26" s="59"/>
+      <c r="E26" s="59"/>
+      <c r="F26" s="59"/>
+      <c r="G26" s="59"/>
+      <c r="H26" s="59"/>
+      <c r="I26" s="30"/>
+      <c r="J26" s="32"/>
+      <c r="K26" s="30"/>
+      <c r="L26" s="30"/>
+      <c r="M26" s="30"/>
+      <c r="N26" s="30"/>
+      <c r="O26" s="30"/>
+      <c r="P26" s="30"/>
     </row>
     <row r="27" spans="1:16" s="2" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="74" t="s">
+      <c r="A27" s="47" t="s">
         <v>63</v>
       </c>
-      <c r="B27" s="75"/>
-      <c r="C27" s="69" t="s">
+      <c r="B27" s="48"/>
+      <c r="C27" s="55" t="s">
         <v>14</v>
       </c>
-      <c r="D27" s="69"/>
-      <c r="E27" s="69"/>
-      <c r="F27" s="69"/>
-      <c r="G27" s="69"/>
-      <c r="H27" s="69"/>
-      <c r="I27" s="31"/>
-      <c r="J27" s="33"/>
-      <c r="K27" s="31"/>
-      <c r="L27" s="31"/>
-      <c r="M27" s="31"/>
-      <c r="N27" s="31"/>
-      <c r="O27" s="31"/>
-      <c r="P27" s="31"/>
+      <c r="D27" s="55"/>
+      <c r="E27" s="55"/>
+      <c r="F27" s="55"/>
+      <c r="G27" s="55"/>
+      <c r="H27" s="55"/>
+      <c r="I27" s="30"/>
+      <c r="J27" s="32"/>
+      <c r="K27" s="30"/>
+      <c r="L27" s="30"/>
+      <c r="M27" s="30"/>
+      <c r="N27" s="30"/>
+      <c r="O27" s="30"/>
+      <c r="P27" s="30"/>
     </row>
     <row r="28" spans="1:16" s="2" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="74" t="s">
+      <c r="A28" s="47" t="s">
         <v>50</v>
       </c>
-      <c r="B28" s="75"/>
-      <c r="C28" s="85" t="s">
+      <c r="B28" s="48"/>
+      <c r="C28" s="49" t="s">
         <v>51</v>
       </c>
-      <c r="D28" s="86"/>
-      <c r="E28" s="86"/>
-      <c r="F28" s="86"/>
-      <c r="G28" s="86"/>
-      <c r="H28" s="87"/>
-      <c r="J28" s="33"/>
-      <c r="K28" s="31"/>
-      <c r="L28" s="31"/>
-      <c r="M28" s="31"/>
-      <c r="N28" s="31"/>
-      <c r="O28" s="31"/>
-      <c r="P28" s="31"/>
+      <c r="D28" s="50"/>
+      <c r="E28" s="50"/>
+      <c r="F28" s="50"/>
+      <c r="G28" s="50"/>
+      <c r="H28" s="51"/>
+      <c r="J28" s="32"/>
+      <c r="K28" s="30"/>
+      <c r="L28" s="30"/>
+      <c r="M28" s="30"/>
+      <c r="N28" s="30"/>
+      <c r="O28" s="30"/>
+      <c r="P28" s="30"/>
     </row>
     <row r="29" spans="1:16" s="2" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="74" t="s">
+      <c r="A29" s="47" t="s">
         <v>64</v>
       </c>
-      <c r="B29" s="75"/>
-      <c r="C29" s="70" t="s">
+      <c r="B29" s="48"/>
+      <c r="C29" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="D29" s="70"/>
-      <c r="E29" s="70"/>
-      <c r="F29" s="70"/>
-      <c r="G29" s="70"/>
-      <c r="H29" s="70"/>
-      <c r="I29" s="31"/>
-      <c r="K29" s="31"/>
-      <c r="L29" s="31"/>
-      <c r="M29" s="31"/>
-      <c r="N29" s="31"/>
-      <c r="O29" s="31"/>
-      <c r="P29" s="31"/>
+      <c r="D29" s="59"/>
+      <c r="E29" s="59"/>
+      <c r="F29" s="59"/>
+      <c r="G29" s="59"/>
+      <c r="H29" s="59"/>
+      <c r="I29" s="30"/>
+      <c r="K29" s="30"/>
+      <c r="L29" s="30"/>
+      <c r="M29" s="30"/>
+      <c r="N29" s="30"/>
+      <c r="O29" s="30"/>
+      <c r="P29" s="30"/>
     </row>
     <row r="30" spans="1:16" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="74" t="s">
+      <c r="A30" s="47" t="s">
         <v>65</v>
       </c>
-      <c r="B30" s="75"/>
-      <c r="C30" s="69" t="s">
+      <c r="B30" s="48"/>
+      <c r="C30" s="55" t="s">
         <v>52</v>
       </c>
-      <c r="D30" s="69"/>
-      <c r="E30" s="69"/>
-      <c r="F30" s="69"/>
-      <c r="G30" s="69"/>
-      <c r="H30" s="69"/>
-      <c r="I30" s="31"/>
-      <c r="J30" s="33"/>
-      <c r="K30" s="31"/>
-      <c r="L30" s="31"/>
-      <c r="M30" s="31"/>
-      <c r="N30" s="31"/>
-      <c r="O30" s="31"/>
-      <c r="P30" s="31"/>
+      <c r="D30" s="55"/>
+      <c r="E30" s="55"/>
+      <c r="F30" s="55"/>
+      <c r="G30" s="55"/>
+      <c r="H30" s="55"/>
+      <c r="I30" s="30"/>
+      <c r="J30" s="32"/>
+      <c r="K30" s="30"/>
+      <c r="L30" s="30"/>
+      <c r="M30" s="30"/>
+      <c r="N30" s="30"/>
+      <c r="O30" s="30"/>
+      <c r="P30" s="30"/>
     </row>
     <row r="31" spans="1:16" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="74" t="s">
+      <c r="A31" s="47" t="s">
         <v>66</v>
       </c>
-      <c r="B31" s="75"/>
-      <c r="C31" s="69" t="s">
+      <c r="B31" s="48"/>
+      <c r="C31" s="55" t="s">
         <v>16</v>
       </c>
-      <c r="D31" s="69"/>
-      <c r="E31" s="69"/>
-      <c r="F31" s="69"/>
-      <c r="G31" s="69"/>
-      <c r="H31" s="69"/>
-      <c r="I31" s="31"/>
-      <c r="J31" s="33"/>
-      <c r="K31" s="31"/>
-      <c r="L31" s="31"/>
-      <c r="M31" s="31"/>
-      <c r="N31" s="31"/>
-      <c r="O31" s="31"/>
-      <c r="P31" s="31"/>
+      <c r="D31" s="55"/>
+      <c r="E31" s="55"/>
+      <c r="F31" s="55"/>
+      <c r="G31" s="55"/>
+      <c r="H31" s="55"/>
+      <c r="I31" s="30"/>
+      <c r="J31" s="32"/>
+      <c r="K31" s="30"/>
+      <c r="L31" s="30"/>
+      <c r="M31" s="30"/>
+      <c r="N31" s="30"/>
+      <c r="O31" s="30"/>
+      <c r="P31" s="30"/>
     </row>
     <row r="32" spans="1:16" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="74" t="s">
+      <c r="A32" s="47" t="s">
         <v>54</v>
       </c>
-      <c r="B32" s="75"/>
-      <c r="C32" s="69" t="s">
+      <c r="B32" s="48"/>
+      <c r="C32" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="D32" s="69"/>
-      <c r="E32" s="69"/>
-      <c r="F32" s="69"/>
-      <c r="G32" s="69"/>
-      <c r="H32" s="69"/>
-      <c r="I32" s="31"/>
-      <c r="J32" s="33"/>
-      <c r="K32" s="31"/>
-      <c r="L32" s="31"/>
-      <c r="M32" s="31"/>
-      <c r="N32" s="31"/>
-      <c r="O32" s="31"/>
-      <c r="P32" s="31"/>
+      <c r="D32" s="55"/>
+      <c r="E32" s="55"/>
+      <c r="F32" s="55"/>
+      <c r="G32" s="55"/>
+      <c r="H32" s="55"/>
+      <c r="I32" s="30"/>
+      <c r="J32" s="32"/>
+      <c r="K32" s="30"/>
+      <c r="L32" s="30"/>
+      <c r="M32" s="30"/>
+      <c r="N32" s="30"/>
+      <c r="O32" s="30"/>
+      <c r="P32" s="30"/>
     </row>
     <row r="33" spans="1:16" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="74" t="s">
+      <c r="A33" s="47" t="s">
         <v>67</v>
       </c>
-      <c r="B33" s="75"/>
-      <c r="C33" s="69" t="s">
+      <c r="B33" s="48"/>
+      <c r="C33" s="55" t="s">
         <v>53</v>
       </c>
-      <c r="D33" s="69"/>
-      <c r="E33" s="69"/>
-      <c r="F33" s="69"/>
-      <c r="G33" s="69"/>
-      <c r="H33" s="69"/>
-      <c r="I33" s="31"/>
-      <c r="J33" s="33"/>
-      <c r="K33" s="31"/>
-      <c r="L33" s="31"/>
-      <c r="M33" s="31"/>
-      <c r="N33" s="31"/>
-      <c r="O33" s="31"/>
-      <c r="P33" s="31"/>
+      <c r="D33" s="55"/>
+      <c r="E33" s="55"/>
+      <c r="F33" s="55"/>
+      <c r="G33" s="55"/>
+      <c r="H33" s="55"/>
+      <c r="I33" s="30"/>
+      <c r="J33" s="32"/>
+      <c r="K33" s="30"/>
+      <c r="L33" s="30"/>
+      <c r="M33" s="30"/>
+      <c r="N33" s="30"/>
+      <c r="O33" s="30"/>
+      <c r="P33" s="30"/>
     </row>
     <row r="34" spans="1:16" s="2" customFormat="1" ht="67.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="38" t="s">
+      <c r="A34" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="B34" s="39"/>
-      <c r="C34" s="39"/>
-      <c r="D34" s="39"/>
-      <c r="E34" s="39"/>
-      <c r="F34" s="39"/>
-      <c r="G34" s="39"/>
-      <c r="H34" s="40"/>
-      <c r="I34" s="31"/>
-      <c r="J34" s="33"/>
-      <c r="K34" s="31"/>
-      <c r="L34" s="31"/>
-      <c r="M34" s="31"/>
-      <c r="N34" s="31"/>
-      <c r="O34" s="31"/>
-      <c r="P34" s="31"/>
+      <c r="B34" s="38"/>
+      <c r="C34" s="38"/>
+      <c r="D34" s="38"/>
+      <c r="E34" s="38"/>
+      <c r="F34" s="38"/>
+      <c r="G34" s="38"/>
+      <c r="H34" s="39"/>
+      <c r="I34" s="30"/>
+      <c r="J34" s="32"/>
+      <c r="K34" s="30"/>
+      <c r="L34" s="30"/>
+      <c r="M34" s="30"/>
+      <c r="N34" s="30"/>
+      <c r="O34" s="30"/>
+      <c r="P34" s="30"/>
     </row>
     <row r="35" spans="1:16" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="88" t="s">
+      <c r="A35" s="52" t="s">
         <v>47</v>
       </c>
-      <c r="B35" s="89"/>
-      <c r="C35" s="89"/>
-      <c r="D35" s="89"/>
-      <c r="E35" s="89"/>
-      <c r="F35" s="89"/>
-      <c r="G35" s="89"/>
-      <c r="H35" s="90"/>
-      <c r="I35" s="31"/>
-      <c r="J35" s="33"/>
-      <c r="K35" s="31"/>
-      <c r="L35" s="31"/>
-      <c r="M35" s="31"/>
-      <c r="N35" s="31"/>
-      <c r="O35" s="31"/>
-      <c r="P35" s="31"/>
+      <c r="B35" s="53"/>
+      <c r="C35" s="53"/>
+      <c r="D35" s="53"/>
+      <c r="E35" s="53"/>
+      <c r="F35" s="53"/>
+      <c r="G35" s="53"/>
+      <c r="H35" s="54"/>
+      <c r="I35" s="30"/>
+      <c r="J35" s="32"/>
+      <c r="K35" s="30"/>
+      <c r="L35" s="30"/>
+      <c r="M35" s="30"/>
+      <c r="N35" s="30"/>
+      <c r="O35" s="30"/>
+      <c r="P35" s="30"/>
     </row>
     <row r="36" spans="1:16" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="79" t="s">
+      <c r="A36" s="56" t="s">
         <v>48</v>
       </c>
-      <c r="B36" s="80"/>
-      <c r="C36" s="80"/>
-      <c r="D36" s="80"/>
-      <c r="E36" s="80"/>
-      <c r="F36" s="80"/>
-      <c r="G36" s="80"/>
-      <c r="H36" s="81"/>
-      <c r="I36" s="31"/>
-      <c r="J36" s="33"/>
-      <c r="K36" s="31"/>
-      <c r="L36" s="31"/>
-      <c r="M36" s="31"/>
-      <c r="N36" s="31"/>
-      <c r="O36" s="31"/>
-      <c r="P36" s="31"/>
+      <c r="B36" s="57"/>
+      <c r="C36" s="57"/>
+      <c r="D36" s="57"/>
+      <c r="E36" s="57"/>
+      <c r="F36" s="57"/>
+      <c r="G36" s="57"/>
+      <c r="H36" s="58"/>
+      <c r="I36" s="30"/>
+      <c r="J36" s="32"/>
+      <c r="K36" s="30"/>
+      <c r="L36" s="30"/>
+      <c r="M36" s="30"/>
+      <c r="N36" s="30"/>
+      <c r="O36" s="30"/>
+      <c r="P36" s="30"/>
     </row>
     <row r="37" spans="1:16" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="82" t="s">
+      <c r="A37" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="B37" s="83"/>
-      <c r="C37" s="83"/>
-      <c r="D37" s="83"/>
-      <c r="E37" s="83"/>
-      <c r="F37" s="83"/>
-      <c r="G37" s="83"/>
-      <c r="H37" s="84"/>
+      <c r="B37" s="45"/>
+      <c r="C37" s="45"/>
+      <c r="D37" s="45"/>
+      <c r="E37" s="45"/>
+      <c r="F37" s="45"/>
+      <c r="G37" s="45"/>
+      <c r="H37" s="46"/>
     </row>
     <row r="38" spans="1:16" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="82" t="s">
+      <c r="A38" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="B38" s="83"/>
-      <c r="C38" s="83"/>
-      <c r="D38" s="83"/>
-      <c r="E38" s="83"/>
-      <c r="F38" s="83"/>
-      <c r="G38" s="83"/>
-      <c r="H38" s="84"/>
+      <c r="B38" s="45"/>
+      <c r="C38" s="45"/>
+      <c r="D38" s="45"/>
+      <c r="E38" s="45"/>
+      <c r="F38" s="45"/>
+      <c r="G38" s="45"/>
+      <c r="H38" s="46"/>
     </row>
     <row r="39" spans="1:16" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A39" s="25"/>
-      <c r="B39" s="26"/>
-      <c r="C39" s="26"/>
-      <c r="D39" s="26"/>
-      <c r="E39" s="26"/>
-      <c r="F39" s="26"/>
-      <c r="G39" s="26"/>
-      <c r="H39" s="27"/>
+      <c r="A39" s="24"/>
+      <c r="B39" s="25"/>
+      <c r="C39" s="25"/>
+      <c r="D39" s="25"/>
+      <c r="E39" s="25"/>
+      <c r="F39" s="25"/>
+      <c r="G39" s="25"/>
+      <c r="H39" s="26"/>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B41" s="28"/>
-      <c r="C41" s="28"/>
-      <c r="D41" s="28"/>
-      <c r="E41" s="28"/>
-      <c r="F41" s="28"/>
-      <c r="G41" s="28"/>
-      <c r="H41" s="28"/>
+      <c r="B41" s="27"/>
+      <c r="C41" s="27"/>
+      <c r="D41" s="27"/>
+      <c r="E41" s="27"/>
+      <c r="F41" s="27"/>
+      <c r="G41" s="27"/>
+      <c r="H41" s="27"/>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B42" s="28"/>
-      <c r="C42" s="28"/>
-      <c r="D42" s="28"/>
-      <c r="E42" s="28"/>
-      <c r="F42" s="28"/>
-      <c r="G42" s="28"/>
-      <c r="H42" s="28"/>
+      <c r="B42" s="27"/>
+      <c r="C42" s="27"/>
+      <c r="D42" s="27"/>
+      <c r="E42" s="27"/>
+      <c r="F42" s="27"/>
+      <c r="G42" s="27"/>
+      <c r="H42" s="27"/>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B43" s="28"/>
-      <c r="C43" s="28"/>
-      <c r="D43" s="28"/>
-      <c r="E43" s="28"/>
-      <c r="F43" s="28"/>
-      <c r="G43" s="28"/>
-      <c r="H43" s="28"/>
+      <c r="B43" s="27"/>
+      <c r="C43" s="27"/>
+      <c r="D43" s="27"/>
+      <c r="E43" s="27"/>
+      <c r="F43" s="27"/>
+      <c r="G43" s="27"/>
+      <c r="H43" s="27"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="51">
-    <mergeCell ref="A37:H37"/>
-    <mergeCell ref="A38:H38"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="C28:H28"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A35:H35"/>
-    <mergeCell ref="C31:H31"/>
-    <mergeCell ref="C32:H32"/>
-    <mergeCell ref="C33:H33"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A36:H36"/>
-    <mergeCell ref="C26:H26"/>
-    <mergeCell ref="C27:H27"/>
-    <mergeCell ref="C29:H29"/>
-    <mergeCell ref="C30:H30"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A18:H18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A17:H17"/>
-    <mergeCell ref="C19:H19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="C20:H20"/>
-    <mergeCell ref="C21:H21"/>
-    <mergeCell ref="C22:H22"/>
-    <mergeCell ref="C23:H23"/>
-    <mergeCell ref="C24:H24"/>
-    <mergeCell ref="C25:H25"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A12:H12"/>
     <mergeCell ref="D5:F11"/>
@@ -2292,6 +2245,42 @@
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B3:H3"/>
+    <mergeCell ref="C21:H21"/>
+    <mergeCell ref="C22:H22"/>
+    <mergeCell ref="C23:H23"/>
+    <mergeCell ref="C24:H24"/>
+    <mergeCell ref="C25:H25"/>
+    <mergeCell ref="A18:H18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A17:H17"/>
+    <mergeCell ref="C19:H19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="C20:H20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A36:H36"/>
+    <mergeCell ref="C26:H26"/>
+    <mergeCell ref="C27:H27"/>
+    <mergeCell ref="C29:H29"/>
+    <mergeCell ref="C30:H30"/>
+    <mergeCell ref="A37:H37"/>
+    <mergeCell ref="A38:H38"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="C28:H28"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A35:H35"/>
+    <mergeCell ref="C31:H31"/>
+    <mergeCell ref="C32:H32"/>
+    <mergeCell ref="C33:H33"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.43307086614173229" right="0.43307086614173229" top="0.51181102362204722" bottom="0.51181102362204722" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>

<commit_message>
For Push Problem CheckIn
</commit_message>
<xml_diff>
--- a/NtierMvc/App_Data/Documents/Excel/QuotePreparation.xlsx
+++ b/NtierMvc/App_Data/Documents/Excel/QuotePreparation.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Deepak\Downloads\C#\NtierMvc\App_Data\Documents\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{643219A6-91D6-4CCC-9A30-92E6F53D6CDA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6DA82B0-B08F-4A75-9E4C-5B78C47F0A38}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -280,13 +280,13 @@
     <t>Price quoted is in #Currency and Ex-Factory.  The rates will vary if the quantity change. The quoted rates are valid only if the quantity is ordered as mentioned in qute. The above mentioned rates are excluding any taxes or charges applicable in case of domestic (IGST as applicable) &amp; Overseas customers (Import duties) purchase which customer has to be borne by Customer at the time of delivery.</t>
   </si>
   <si>
-    <t>Amount in Words: #AmountInWords only</t>
-  </si>
-  <si>
     <t>#CustomerAddress1</t>
   </si>
   <si>
     <t>#CustomerAddress2</t>
+  </si>
+  <si>
+    <t>Amount in Words: #AmountInWords</t>
   </si>
 </sst>
 </file>
@@ -638,7 +638,7 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
@@ -701,10 +701,6 @@
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -785,10 +781,6 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -803,9 +795,6 @@
     </xf>
     <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1391,8 +1380,8 @@
   </sheetPr>
   <dimension ref="A1:P43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1405,266 +1394,266 @@
     <col min="6" max="6" width="19.28515625" style="1" customWidth="1"/>
     <col min="7" max="7" width="25.42578125" style="1" customWidth="1"/>
     <col min="8" max="8" width="26.85546875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="32"/>
-    <col min="10" max="10" width="9.140625" style="37"/>
-    <col min="11" max="16" width="9.140625" style="32"/>
+    <col min="9" max="9" width="9.140625" style="31"/>
+    <col min="10" max="10" width="9.140625" style="36"/>
+    <col min="11" max="16" width="9.140625" style="31"/>
     <col min="17" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="47" t="s">
+    <row r="1" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="30"/>
-      <c r="N1" s="30"/>
-      <c r="O1" s="30"/>
-      <c r="P1" s="30"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29"/>
+      <c r="O1" s="29"/>
+      <c r="P1" s="29"/>
     </row>
     <row r="2" spans="1:16" s="4" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="64"/>
-      <c r="B2" s="61" t="s">
+      <c r="A2" s="61"/>
+      <c r="B2" s="58" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62"/>
-      <c r="F2" s="62"/>
-      <c r="G2" s="62"/>
-      <c r="H2" s="63"/>
-      <c r="J2" s="36"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="60"/>
+      <c r="J2" s="35"/>
     </row>
     <row r="3" spans="1:16" s="4" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="65"/>
-      <c r="B3" s="66" t="s">
+      <c r="A3" s="62"/>
+      <c r="B3" s="63" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="67"/>
-      <c r="D3" s="67"/>
-      <c r="E3" s="67"/>
-      <c r="F3" s="67"/>
-      <c r="G3" s="67"/>
-      <c r="H3" s="68"/>
-      <c r="J3" s="33"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
+      <c r="F3" s="64"/>
+      <c r="G3" s="64"/>
+      <c r="H3" s="65"/>
+      <c r="J3" s="32"/>
     </row>
     <row r="4" spans="1:16" s="4" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="51" t="s">
+      <c r="A4" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="B4" s="51"/>
-      <c r="C4" s="51"/>
-      <c r="D4" s="48" t="s">
+      <c r="B4" s="48"/>
+      <c r="C4" s="48"/>
+      <c r="D4" s="45" t="s">
         <v>39</v>
       </c>
-      <c r="E4" s="48"/>
-      <c r="F4" s="48"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
       <c r="G4" s="3" t="s">
         <v>38</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="I4" s="31"/>
-      <c r="J4" s="33"/>
-      <c r="K4" s="31"/>
-      <c r="L4" s="31"/>
-      <c r="M4" s="31"/>
-      <c r="N4" s="31"/>
-      <c r="O4" s="31"/>
-      <c r="P4" s="31"/>
+      <c r="I4" s="30"/>
+      <c r="J4" s="32"/>
+      <c r="K4" s="30"/>
+      <c r="L4" s="30"/>
+      <c r="M4" s="30"/>
+      <c r="N4" s="30"/>
+      <c r="O4" s="30"/>
+      <c r="P4" s="30"/>
     </row>
     <row r="5" spans="1:16" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="52"/>
-      <c r="B5" s="53"/>
-      <c r="C5" s="54"/>
-      <c r="D5" s="49" t="s">
+      <c r="A5" s="49"/>
+      <c r="B5" s="50"/>
+      <c r="C5" s="51"/>
+      <c r="D5" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="E5" s="50"/>
-      <c r="F5" s="50"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="47"/>
       <c r="G5" s="5" t="s">
         <v>6</v>
       </c>
       <c r="H5" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="I5" s="31"/>
-      <c r="J5" s="33"/>
-      <c r="K5" s="31"/>
-      <c r="L5" s="31"/>
-      <c r="M5" s="31"/>
-      <c r="N5" s="31"/>
-      <c r="O5" s="31"/>
-      <c r="P5" s="31"/>
+      <c r="I5" s="30"/>
+      <c r="J5" s="32"/>
+      <c r="K5" s="30"/>
+      <c r="L5" s="30"/>
+      <c r="M5" s="30"/>
+      <c r="N5" s="30"/>
+      <c r="O5" s="30"/>
+      <c r="P5" s="30"/>
     </row>
     <row r="6" spans="1:16" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="55" t="s">
+      <c r="A6" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="56"/>
-      <c r="C6" s="57"/>
-      <c r="D6" s="49"/>
-      <c r="E6" s="50"/>
-      <c r="F6" s="50"/>
+      <c r="B6" s="53"/>
+      <c r="C6" s="54"/>
+      <c r="D6" s="46"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="47"/>
       <c r="G6" s="5" t="s">
         <v>7</v>
       </c>
       <c r="H6" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="I6" s="31"/>
-      <c r="J6" s="33"/>
-      <c r="K6" s="31"/>
-      <c r="L6" s="31"/>
-      <c r="M6" s="31"/>
-      <c r="N6" s="31"/>
-      <c r="O6" s="31"/>
-      <c r="P6" s="31"/>
+      <c r="I6" s="30"/>
+      <c r="J6" s="32"/>
+      <c r="K6" s="30"/>
+      <c r="L6" s="30"/>
+      <c r="M6" s="30"/>
+      <c r="N6" s="30"/>
+      <c r="O6" s="30"/>
+      <c r="P6" s="30"/>
     </row>
     <row r="7" spans="1:16" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="55" t="s">
-        <v>71</v>
-      </c>
-      <c r="B7" s="56"/>
-      <c r="C7" s="57"/>
-      <c r="D7" s="49"/>
-      <c r="E7" s="50"/>
-      <c r="F7" s="50"/>
+      <c r="A7" s="52" t="s">
+        <v>70</v>
+      </c>
+      <c r="B7" s="53"/>
+      <c r="C7" s="54"/>
+      <c r="D7" s="46"/>
+      <c r="E7" s="47"/>
+      <c r="F7" s="47"/>
       <c r="G7" s="5" t="s">
         <v>17</v>
       </c>
       <c r="H7" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="I7" s="31"/>
-      <c r="J7" s="33"/>
-      <c r="K7" s="31"/>
-      <c r="L7" s="31"/>
-      <c r="M7" s="31"/>
-      <c r="N7" s="31"/>
-      <c r="O7" s="31"/>
-      <c r="P7" s="31"/>
+      <c r="I7" s="30"/>
+      <c r="J7" s="32"/>
+      <c r="K7" s="30"/>
+      <c r="L7" s="30"/>
+      <c r="M7" s="30"/>
+      <c r="N7" s="30"/>
+      <c r="O7" s="30"/>
+      <c r="P7" s="30"/>
     </row>
     <row r="8" spans="1:16" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="55" t="s">
-        <v>72</v>
-      </c>
-      <c r="B8" s="56"/>
-      <c r="C8" s="57"/>
-      <c r="D8" s="49"/>
-      <c r="E8" s="50"/>
-      <c r="F8" s="50"/>
+      <c r="A8" s="52" t="s">
+        <v>71</v>
+      </c>
+      <c r="B8" s="53"/>
+      <c r="C8" s="54"/>
+      <c r="D8" s="46"/>
+      <c r="E8" s="47"/>
+      <c r="F8" s="47"/>
       <c r="G8" s="5" t="s">
         <v>19</v>
       </c>
       <c r="H8" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="I8" s="31"/>
-      <c r="J8" s="33"/>
-      <c r="K8" s="31"/>
-      <c r="L8" s="31"/>
-      <c r="M8" s="31"/>
-      <c r="N8" s="31"/>
-      <c r="O8" s="31"/>
-      <c r="P8" s="31"/>
+      <c r="I8" s="30"/>
+      <c r="J8" s="32"/>
+      <c r="K8" s="30"/>
+      <c r="L8" s="30"/>
+      <c r="M8" s="30"/>
+      <c r="N8" s="30"/>
+      <c r="O8" s="30"/>
+      <c r="P8" s="30"/>
     </row>
     <row r="9" spans="1:16" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="55" t="s">
+      <c r="A9" s="52" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="56"/>
-      <c r="C9" s="57"/>
-      <c r="D9" s="49"/>
-      <c r="E9" s="50"/>
-      <c r="F9" s="50"/>
+      <c r="B9" s="53"/>
+      <c r="C9" s="54"/>
+      <c r="D9" s="46"/>
+      <c r="E9" s="47"/>
+      <c r="F9" s="47"/>
       <c r="G9" s="5" t="s">
         <v>5</v>
       </c>
       <c r="H9" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="I9" s="31"/>
-      <c r="J9" s="33"/>
-      <c r="K9" s="31"/>
-      <c r="L9" s="31"/>
-      <c r="M9" s="31"/>
-      <c r="N9" s="31"/>
-      <c r="O9" s="31"/>
-      <c r="P9" s="31"/>
+      <c r="I9" s="30"/>
+      <c r="J9" s="32"/>
+      <c r="K9" s="30"/>
+      <c r="L9" s="30"/>
+      <c r="M9" s="30"/>
+      <c r="N9" s="30"/>
+      <c r="O9" s="30"/>
+      <c r="P9" s="30"/>
     </row>
     <row r="10" spans="1:16" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="55"/>
-      <c r="B10" s="56"/>
-      <c r="C10" s="57"/>
-      <c r="D10" s="49"/>
-      <c r="E10" s="50"/>
-      <c r="F10" s="50"/>
+      <c r="A10" s="52"/>
+      <c r="B10" s="53"/>
+      <c r="C10" s="54"/>
+      <c r="D10" s="46"/>
+      <c r="E10" s="47"/>
+      <c r="F10" s="47"/>
       <c r="G10" s="5" t="s">
         <v>4</v>
       </c>
       <c r="H10" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="I10" s="31"/>
-      <c r="J10" s="34"/>
-      <c r="K10" s="31"/>
-      <c r="L10" s="31"/>
-      <c r="M10" s="31"/>
-      <c r="N10" s="31"/>
-      <c r="O10" s="31"/>
-      <c r="P10" s="31"/>
+      <c r="I10" s="30"/>
+      <c r="J10" s="33"/>
+      <c r="K10" s="30"/>
+      <c r="L10" s="30"/>
+      <c r="M10" s="30"/>
+      <c r="N10" s="30"/>
+      <c r="O10" s="30"/>
+      <c r="P10" s="30"/>
     </row>
     <row r="11" spans="1:16" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="58"/>
-      <c r="B11" s="59"/>
-      <c r="C11" s="60"/>
-      <c r="D11" s="49"/>
-      <c r="E11" s="50"/>
-      <c r="F11" s="50"/>
+      <c r="A11" s="55"/>
+      <c r="B11" s="56"/>
+      <c r="C11" s="57"/>
+      <c r="D11" s="46"/>
+      <c r="E11" s="47"/>
+      <c r="F11" s="47"/>
       <c r="G11" s="5" t="s">
         <v>11</v>
       </c>
       <c r="H11" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="I11" s="31"/>
-      <c r="J11" s="36"/>
-      <c r="K11" s="31"/>
-      <c r="L11" s="31"/>
-      <c r="M11" s="31"/>
-      <c r="N11" s="31"/>
-      <c r="O11" s="31"/>
-      <c r="P11" s="31"/>
+      <c r="I11" s="30"/>
+      <c r="J11" s="35"/>
+      <c r="K11" s="30"/>
+      <c r="L11" s="30"/>
+      <c r="M11" s="30"/>
+      <c r="N11" s="30"/>
+      <c r="O11" s="30"/>
+      <c r="P11" s="30"/>
     </row>
     <row r="12" spans="1:16" s="4" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="48" t="s">
+      <c r="A12" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="48"/>
-      <c r="C12" s="48"/>
-      <c r="D12" s="48"/>
-      <c r="E12" s="48"/>
-      <c r="F12" s="48"/>
-      <c r="G12" s="48"/>
-      <c r="H12" s="48"/>
-      <c r="I12" s="31"/>
-      <c r="K12" s="31"/>
-      <c r="L12" s="31"/>
-      <c r="M12" s="31"/>
-      <c r="N12" s="31"/>
-      <c r="O12" s="31"/>
-      <c r="P12" s="31"/>
+      <c r="B12" s="45"/>
+      <c r="C12" s="45"/>
+      <c r="D12" s="45"/>
+      <c r="E12" s="45"/>
+      <c r="F12" s="45"/>
+      <c r="G12" s="45"/>
+      <c r="H12" s="45"/>
+      <c r="I12" s="30"/>
+      <c r="K12" s="30"/>
+      <c r="L12" s="30"/>
+      <c r="M12" s="30"/>
+      <c r="N12" s="30"/>
+      <c r="O12" s="30"/>
+      <c r="P12" s="30"/>
     </row>
     <row r="13" spans="1:16" s="4" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
@@ -1691,17 +1680,17 @@
       <c r="H13" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="I13" s="31"/>
-      <c r="J13" s="33"/>
-      <c r="K13" s="31"/>
-      <c r="L13" s="31"/>
-      <c r="M13" s="31"/>
-      <c r="N13" s="31"/>
-      <c r="O13" s="31"/>
-      <c r="P13" s="31"/>
+      <c r="I13" s="30"/>
+      <c r="J13" s="32"/>
+      <c r="K13" s="30"/>
+      <c r="L13" s="30"/>
+      <c r="M13" s="30"/>
+      <c r="N13" s="30"/>
+      <c r="O13" s="30"/>
+      <c r="P13" s="30"/>
     </row>
     <row r="14" spans="1:16" s="4" customFormat="1" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A14" s="41"/>
+      <c r="A14" s="13"/>
       <c r="B14" s="13"/>
       <c r="C14" s="14"/>
       <c r="D14" s="15"/>
@@ -1709,534 +1698,534 @@
       <c r="F14" s="16"/>
       <c r="G14" s="16"/>
       <c r="H14" s="13"/>
-      <c r="I14" s="31"/>
-      <c r="J14" s="33"/>
-      <c r="K14" s="31"/>
-      <c r="L14" s="31"/>
-      <c r="M14" s="31"/>
-      <c r="N14" s="31"/>
-      <c r="O14" s="31"/>
-      <c r="P14" s="31"/>
+      <c r="I14" s="30"/>
+      <c r="J14" s="32"/>
+      <c r="K14" s="30"/>
+      <c r="L14" s="30"/>
+      <c r="M14" s="30"/>
+      <c r="N14" s="30"/>
+      <c r="O14" s="30"/>
+      <c r="P14" s="30"/>
     </row>
     <row r="15" spans="1:16" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A15" s="46"/>
-      <c r="B15" s="42"/>
-      <c r="C15" s="43"/>
-      <c r="D15" s="42"/>
-      <c r="E15" s="42"/>
-      <c r="F15" s="44"/>
-      <c r="G15" s="45"/>
-      <c r="H15" s="42"/>
-    </row>
-    <row r="16" spans="1:16" s="24" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="17"/>
-      <c r="B16" s="18"/>
-      <c r="C16" s="19" t="s">
+      <c r="A15" s="13"/>
+      <c r="B15" s="40"/>
+      <c r="C15" s="41"/>
+      <c r="D15" s="40"/>
+      <c r="E15" s="40"/>
+      <c r="F15" s="42"/>
+      <c r="G15" s="43"/>
+      <c r="H15" s="40"/>
+    </row>
+    <row r="16" spans="1:16" s="23" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="13"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="D16" s="20"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="22" t="s">
+      <c r="D16" s="19"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="H16" s="23"/>
-      <c r="I16" s="33"/>
-      <c r="J16" s="33"/>
-      <c r="K16" s="33"/>
-      <c r="L16" s="33"/>
-      <c r="M16" s="33"/>
-      <c r="N16" s="33"/>
-      <c r="O16" s="33"/>
-      <c r="P16" s="33"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="32"/>
+      <c r="J16" s="32"/>
+      <c r="K16" s="32"/>
+      <c r="L16" s="32"/>
+      <c r="M16" s="32"/>
+      <c r="N16" s="32"/>
+      <c r="O16" s="32"/>
+      <c r="P16" s="32"/>
     </row>
     <row r="17" spans="1:16" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="76" t="s">
-        <v>70</v>
-      </c>
-      <c r="B17" s="77"/>
-      <c r="C17" s="77"/>
-      <c r="D17" s="77"/>
-      <c r="E17" s="77"/>
-      <c r="F17" s="77"/>
-      <c r="G17" s="77"/>
-      <c r="H17" s="78"/>
-      <c r="J17" s="33"/>
-      <c r="K17" s="31"/>
-      <c r="L17" s="31"/>
-      <c r="M17" s="31"/>
-      <c r="N17" s="31"/>
-      <c r="O17" s="31"/>
-      <c r="P17" s="31"/>
+      <c r="A17" s="73" t="s">
+        <v>72</v>
+      </c>
+      <c r="B17" s="74"/>
+      <c r="C17" s="74"/>
+      <c r="D17" s="74"/>
+      <c r="E17" s="74"/>
+      <c r="F17" s="74"/>
+      <c r="G17" s="74"/>
+      <c r="H17" s="75"/>
+      <c r="J17" s="32"/>
+      <c r="K17" s="30"/>
+      <c r="L17" s="30"/>
+      <c r="M17" s="30"/>
+      <c r="N17" s="30"/>
+      <c r="O17" s="30"/>
+      <c r="P17" s="30"/>
     </row>
     <row r="18" spans="1:16" s="2" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="71" t="s">
+      <c r="A18" s="68" t="s">
         <v>0</v>
       </c>
-      <c r="B18" s="72"/>
-      <c r="C18" s="72"/>
-      <c r="D18" s="72"/>
-      <c r="E18" s="72"/>
-      <c r="F18" s="72"/>
-      <c r="G18" s="72"/>
-      <c r="H18" s="73"/>
-      <c r="I18" s="31"/>
-      <c r="J18" s="33"/>
-      <c r="K18" s="31"/>
-      <c r="L18" s="31"/>
-      <c r="M18" s="31"/>
-      <c r="N18" s="31"/>
-      <c r="O18" s="31"/>
-      <c r="P18" s="31"/>
+      <c r="B18" s="69"/>
+      <c r="C18" s="69"/>
+      <c r="D18" s="69"/>
+      <c r="E18" s="69"/>
+      <c r="F18" s="69"/>
+      <c r="G18" s="69"/>
+      <c r="H18" s="70"/>
+      <c r="I18" s="30"/>
+      <c r="J18" s="32"/>
+      <c r="K18" s="30"/>
+      <c r="L18" s="30"/>
+      <c r="M18" s="30"/>
+      <c r="N18" s="30"/>
+      <c r="O18" s="30"/>
+      <c r="P18" s="30"/>
     </row>
     <row r="19" spans="1:16" s="2" customFormat="1" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="74" t="s">
+      <c r="A19" s="71" t="s">
         <v>55</v>
       </c>
-      <c r="B19" s="75"/>
-      <c r="C19" s="70" t="s">
+      <c r="B19" s="72"/>
+      <c r="C19" s="67" t="s">
         <v>69</v>
       </c>
-      <c r="D19" s="70"/>
-      <c r="E19" s="70"/>
-      <c r="F19" s="70"/>
-      <c r="G19" s="70"/>
-      <c r="H19" s="70"/>
-      <c r="I19" s="31"/>
-      <c r="J19" s="33"/>
-      <c r="K19" s="31"/>
-      <c r="L19" s="31"/>
-      <c r="M19" s="31"/>
-      <c r="N19" s="31"/>
-      <c r="O19" s="31"/>
-      <c r="P19" s="31"/>
+      <c r="D19" s="67"/>
+      <c r="E19" s="67"/>
+      <c r="F19" s="67"/>
+      <c r="G19" s="67"/>
+      <c r="H19" s="67"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="32"/>
+      <c r="K19" s="30"/>
+      <c r="L19" s="30"/>
+      <c r="M19" s="30"/>
+      <c r="N19" s="30"/>
+      <c r="O19" s="30"/>
+      <c r="P19" s="30"/>
     </row>
     <row r="20" spans="1:16" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="74" t="s">
+      <c r="A20" s="71" t="s">
         <v>56</v>
       </c>
-      <c r="B20" s="75"/>
-      <c r="C20" s="69" t="s">
+      <c r="B20" s="72"/>
+      <c r="C20" s="66" t="s">
         <v>68</v>
       </c>
-      <c r="D20" s="69"/>
-      <c r="E20" s="69"/>
-      <c r="F20" s="69"/>
-      <c r="G20" s="69"/>
-      <c r="H20" s="69"/>
-      <c r="I20" s="31"/>
-      <c r="J20" s="33"/>
-      <c r="K20" s="31"/>
-      <c r="L20" s="31"/>
-      <c r="M20" s="31"/>
-      <c r="N20" s="31"/>
-      <c r="O20" s="31"/>
-      <c r="P20" s="31"/>
+      <c r="D20" s="66"/>
+      <c r="E20" s="66"/>
+      <c r="F20" s="66"/>
+      <c r="G20" s="66"/>
+      <c r="H20" s="66"/>
+      <c r="I20" s="30"/>
+      <c r="J20" s="32"/>
+      <c r="K20" s="30"/>
+      <c r="L20" s="30"/>
+      <c r="M20" s="30"/>
+      <c r="N20" s="30"/>
+      <c r="O20" s="30"/>
+      <c r="P20" s="30"/>
     </row>
     <row r="21" spans="1:16" s="2" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="74" t="s">
+      <c r="A21" s="71" t="s">
         <v>57</v>
       </c>
-      <c r="B21" s="75"/>
-      <c r="C21" s="69" t="s">
+      <c r="B21" s="72"/>
+      <c r="C21" s="66" t="s">
         <v>34</v>
       </c>
-      <c r="D21" s="69"/>
-      <c r="E21" s="69"/>
-      <c r="F21" s="69"/>
-      <c r="G21" s="69"/>
-      <c r="H21" s="69"/>
-      <c r="I21" s="31"/>
-      <c r="J21" s="33"/>
-      <c r="K21" s="31"/>
-      <c r="L21" s="31"/>
-      <c r="M21" s="31"/>
-      <c r="N21" s="31"/>
-      <c r="O21" s="31"/>
-      <c r="P21" s="31"/>
+      <c r="D21" s="66"/>
+      <c r="E21" s="66"/>
+      <c r="F21" s="66"/>
+      <c r="G21" s="66"/>
+      <c r="H21" s="66"/>
+      <c r="I21" s="30"/>
+      <c r="J21" s="32"/>
+      <c r="K21" s="30"/>
+      <c r="L21" s="30"/>
+      <c r="M21" s="30"/>
+      <c r="N21" s="30"/>
+      <c r="O21" s="30"/>
+      <c r="P21" s="30"/>
     </row>
     <row r="22" spans="1:16" s="2" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="74" t="s">
+      <c r="A22" s="71" t="s">
         <v>58</v>
       </c>
-      <c r="B22" s="75"/>
-      <c r="C22" s="69" t="s">
+      <c r="B22" s="72"/>
+      <c r="C22" s="66" t="s">
         <v>29</v>
       </c>
-      <c r="D22" s="69"/>
-      <c r="E22" s="69"/>
-      <c r="F22" s="69"/>
-      <c r="G22" s="69"/>
-      <c r="H22" s="69"/>
-      <c r="I22" s="31"/>
-      <c r="J22" s="33"/>
-      <c r="K22" s="31"/>
-      <c r="L22" s="31"/>
-      <c r="M22" s="31"/>
-      <c r="N22" s="31"/>
-      <c r="O22" s="31"/>
-      <c r="P22" s="31"/>
+      <c r="D22" s="66"/>
+      <c r="E22" s="66"/>
+      <c r="F22" s="66"/>
+      <c r="G22" s="66"/>
+      <c r="H22" s="66"/>
+      <c r="I22" s="30"/>
+      <c r="J22" s="32"/>
+      <c r="K22" s="30"/>
+      <c r="L22" s="30"/>
+      <c r="M22" s="30"/>
+      <c r="N22" s="30"/>
+      <c r="O22" s="30"/>
+      <c r="P22" s="30"/>
     </row>
     <row r="23" spans="1:16" s="2" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="74" t="s">
+      <c r="A23" s="71" t="s">
         <v>59</v>
       </c>
-      <c r="B23" s="75"/>
-      <c r="C23" s="70" t="s">
+      <c r="B23" s="72"/>
+      <c r="C23" s="67" t="s">
         <v>49</v>
       </c>
-      <c r="D23" s="70"/>
-      <c r="E23" s="70"/>
-      <c r="F23" s="70"/>
-      <c r="G23" s="70"/>
-      <c r="H23" s="70"/>
-      <c r="I23" s="31"/>
-      <c r="J23" s="33"/>
-      <c r="K23" s="31"/>
-      <c r="L23" s="31"/>
-      <c r="M23" s="31"/>
-      <c r="N23" s="31"/>
-      <c r="O23" s="31"/>
-      <c r="P23" s="31"/>
+      <c r="D23" s="67"/>
+      <c r="E23" s="67"/>
+      <c r="F23" s="67"/>
+      <c r="G23" s="67"/>
+      <c r="H23" s="67"/>
+      <c r="I23" s="30"/>
+      <c r="J23" s="32"/>
+      <c r="K23" s="30"/>
+      <c r="L23" s="30"/>
+      <c r="M23" s="30"/>
+      <c r="N23" s="30"/>
+      <c r="O23" s="30"/>
+      <c r="P23" s="30"/>
     </row>
     <row r="24" spans="1:16" s="2" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="74" t="s">
+      <c r="A24" s="71" t="s">
         <v>60</v>
       </c>
-      <c r="B24" s="75"/>
-      <c r="C24" s="69" t="s">
+      <c r="B24" s="72"/>
+      <c r="C24" s="66" t="s">
         <v>12</v>
       </c>
-      <c r="D24" s="69"/>
-      <c r="E24" s="69"/>
-      <c r="F24" s="69"/>
-      <c r="G24" s="69"/>
-      <c r="H24" s="69"/>
-      <c r="I24" s="31"/>
-      <c r="J24" s="33"/>
-      <c r="K24" s="31"/>
-      <c r="L24" s="31"/>
-      <c r="M24" s="31"/>
-      <c r="N24" s="31"/>
-      <c r="O24" s="31"/>
-      <c r="P24" s="31"/>
+      <c r="D24" s="66"/>
+      <c r="E24" s="66"/>
+      <c r="F24" s="66"/>
+      <c r="G24" s="66"/>
+      <c r="H24" s="66"/>
+      <c r="I24" s="30"/>
+      <c r="J24" s="32"/>
+      <c r="K24" s="30"/>
+      <c r="L24" s="30"/>
+      <c r="M24" s="30"/>
+      <c r="N24" s="30"/>
+      <c r="O24" s="30"/>
+      <c r="P24" s="30"/>
     </row>
     <row r="25" spans="1:16" s="2" customFormat="1" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A25" s="74" t="s">
+      <c r="A25" s="71" t="s">
         <v>61</v>
       </c>
-      <c r="B25" s="75"/>
-      <c r="C25" s="69" t="s">
+      <c r="B25" s="72"/>
+      <c r="C25" s="66" t="s">
         <v>33</v>
       </c>
-      <c r="D25" s="69"/>
-      <c r="E25" s="69"/>
-      <c r="F25" s="69"/>
-      <c r="G25" s="69"/>
-      <c r="H25" s="69"/>
-      <c r="I25" s="31"/>
-      <c r="J25" s="33"/>
-      <c r="K25" s="31"/>
-      <c r="L25" s="31"/>
-      <c r="M25" s="31"/>
-      <c r="N25" s="31"/>
-      <c r="O25" s="31"/>
-      <c r="P25" s="31"/>
+      <c r="D25" s="66"/>
+      <c r="E25" s="66"/>
+      <c r="F25" s="66"/>
+      <c r="G25" s="66"/>
+      <c r="H25" s="66"/>
+      <c r="I25" s="30"/>
+      <c r="J25" s="32"/>
+      <c r="K25" s="30"/>
+      <c r="L25" s="30"/>
+      <c r="M25" s="30"/>
+      <c r="N25" s="30"/>
+      <c r="O25" s="30"/>
+      <c r="P25" s="30"/>
     </row>
     <row r="26" spans="1:16" s="2" customFormat="1" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A26" s="74" t="s">
+      <c r="A26" s="71" t="s">
         <v>62</v>
       </c>
-      <c r="B26" s="75"/>
-      <c r="C26" s="70" t="s">
+      <c r="B26" s="72"/>
+      <c r="C26" s="67" t="s">
         <v>13</v>
       </c>
-      <c r="D26" s="70"/>
-      <c r="E26" s="70"/>
-      <c r="F26" s="70"/>
-      <c r="G26" s="70"/>
-      <c r="H26" s="70"/>
-      <c r="I26" s="31"/>
-      <c r="J26" s="33"/>
-      <c r="K26" s="31"/>
-      <c r="L26" s="31"/>
-      <c r="M26" s="31"/>
-      <c r="N26" s="31"/>
-      <c r="O26" s="31"/>
-      <c r="P26" s="31"/>
+      <c r="D26" s="67"/>
+      <c r="E26" s="67"/>
+      <c r="F26" s="67"/>
+      <c r="G26" s="67"/>
+      <c r="H26" s="67"/>
+      <c r="I26" s="30"/>
+      <c r="J26" s="32"/>
+      <c r="K26" s="30"/>
+      <c r="L26" s="30"/>
+      <c r="M26" s="30"/>
+      <c r="N26" s="30"/>
+      <c r="O26" s="30"/>
+      <c r="P26" s="30"/>
     </row>
     <row r="27" spans="1:16" s="2" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="74" t="s">
+      <c r="A27" s="71" t="s">
         <v>63</v>
       </c>
-      <c r="B27" s="75"/>
-      <c r="C27" s="69" t="s">
+      <c r="B27" s="72"/>
+      <c r="C27" s="66" t="s">
         <v>14</v>
       </c>
-      <c r="D27" s="69"/>
-      <c r="E27" s="69"/>
-      <c r="F27" s="69"/>
-      <c r="G27" s="69"/>
-      <c r="H27" s="69"/>
-      <c r="I27" s="31"/>
-      <c r="J27" s="33"/>
-      <c r="K27" s="31"/>
-      <c r="L27" s="31"/>
-      <c r="M27" s="31"/>
-      <c r="N27" s="31"/>
-      <c r="O27" s="31"/>
-      <c r="P27" s="31"/>
+      <c r="D27" s="66"/>
+      <c r="E27" s="66"/>
+      <c r="F27" s="66"/>
+      <c r="G27" s="66"/>
+      <c r="H27" s="66"/>
+      <c r="I27" s="30"/>
+      <c r="J27" s="32"/>
+      <c r="K27" s="30"/>
+      <c r="L27" s="30"/>
+      <c r="M27" s="30"/>
+      <c r="N27" s="30"/>
+      <c r="O27" s="30"/>
+      <c r="P27" s="30"/>
     </row>
     <row r="28" spans="1:16" s="2" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="74" t="s">
+      <c r="A28" s="71" t="s">
         <v>50</v>
       </c>
-      <c r="B28" s="75"/>
-      <c r="C28" s="85" t="s">
+      <c r="B28" s="72"/>
+      <c r="C28" s="82" t="s">
         <v>51</v>
       </c>
-      <c r="D28" s="86"/>
-      <c r="E28" s="86"/>
-      <c r="F28" s="86"/>
-      <c r="G28" s="86"/>
-      <c r="H28" s="87"/>
-      <c r="J28" s="33"/>
-      <c r="K28" s="31"/>
-      <c r="L28" s="31"/>
-      <c r="M28" s="31"/>
-      <c r="N28" s="31"/>
-      <c r="O28" s="31"/>
-      <c r="P28" s="31"/>
+      <c r="D28" s="83"/>
+      <c r="E28" s="83"/>
+      <c r="F28" s="83"/>
+      <c r="G28" s="83"/>
+      <c r="H28" s="84"/>
+      <c r="J28" s="32"/>
+      <c r="K28" s="30"/>
+      <c r="L28" s="30"/>
+      <c r="M28" s="30"/>
+      <c r="N28" s="30"/>
+      <c r="O28" s="30"/>
+      <c r="P28" s="30"/>
     </row>
     <row r="29" spans="1:16" s="2" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="74" t="s">
+      <c r="A29" s="71" t="s">
         <v>64</v>
       </c>
-      <c r="B29" s="75"/>
-      <c r="C29" s="70" t="s">
+      <c r="B29" s="72"/>
+      <c r="C29" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="D29" s="70"/>
-      <c r="E29" s="70"/>
-      <c r="F29" s="70"/>
-      <c r="G29" s="70"/>
-      <c r="H29" s="70"/>
-      <c r="I29" s="31"/>
-      <c r="K29" s="31"/>
-      <c r="L29" s="31"/>
-      <c r="M29" s="31"/>
-      <c r="N29" s="31"/>
-      <c r="O29" s="31"/>
-      <c r="P29" s="31"/>
+      <c r="D29" s="67"/>
+      <c r="E29" s="67"/>
+      <c r="F29" s="67"/>
+      <c r="G29" s="67"/>
+      <c r="H29" s="67"/>
+      <c r="I29" s="30"/>
+      <c r="K29" s="30"/>
+      <c r="L29" s="30"/>
+      <c r="M29" s="30"/>
+      <c r="N29" s="30"/>
+      <c r="O29" s="30"/>
+      <c r="P29" s="30"/>
     </row>
     <row r="30" spans="1:16" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="74" t="s">
+      <c r="A30" s="71" t="s">
         <v>65</v>
       </c>
-      <c r="B30" s="75"/>
-      <c r="C30" s="69" t="s">
+      <c r="B30" s="72"/>
+      <c r="C30" s="66" t="s">
         <v>52</v>
       </c>
-      <c r="D30" s="69"/>
-      <c r="E30" s="69"/>
-      <c r="F30" s="69"/>
-      <c r="G30" s="69"/>
-      <c r="H30" s="69"/>
-      <c r="I30" s="31"/>
-      <c r="J30" s="33"/>
-      <c r="K30" s="31"/>
-      <c r="L30" s="31"/>
-      <c r="M30" s="31"/>
-      <c r="N30" s="31"/>
-      <c r="O30" s="31"/>
-      <c r="P30" s="31"/>
+      <c r="D30" s="66"/>
+      <c r="E30" s="66"/>
+      <c r="F30" s="66"/>
+      <c r="G30" s="66"/>
+      <c r="H30" s="66"/>
+      <c r="I30" s="30"/>
+      <c r="J30" s="32"/>
+      <c r="K30" s="30"/>
+      <c r="L30" s="30"/>
+      <c r="M30" s="30"/>
+      <c r="N30" s="30"/>
+      <c r="O30" s="30"/>
+      <c r="P30" s="30"/>
     </row>
     <row r="31" spans="1:16" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="74" t="s">
+      <c r="A31" s="71" t="s">
         <v>66</v>
       </c>
-      <c r="B31" s="75"/>
-      <c r="C31" s="69" t="s">
+      <c r="B31" s="72"/>
+      <c r="C31" s="66" t="s">
         <v>16</v>
       </c>
-      <c r="D31" s="69"/>
-      <c r="E31" s="69"/>
-      <c r="F31" s="69"/>
-      <c r="G31" s="69"/>
-      <c r="H31" s="69"/>
-      <c r="I31" s="31"/>
-      <c r="J31" s="33"/>
-      <c r="K31" s="31"/>
-      <c r="L31" s="31"/>
-      <c r="M31" s="31"/>
-      <c r="N31" s="31"/>
-      <c r="O31" s="31"/>
-      <c r="P31" s="31"/>
+      <c r="D31" s="66"/>
+      <c r="E31" s="66"/>
+      <c r="F31" s="66"/>
+      <c r="G31" s="66"/>
+      <c r="H31" s="66"/>
+      <c r="I31" s="30"/>
+      <c r="J31" s="32"/>
+      <c r="K31" s="30"/>
+      <c r="L31" s="30"/>
+      <c r="M31" s="30"/>
+      <c r="N31" s="30"/>
+      <c r="O31" s="30"/>
+      <c r="P31" s="30"/>
     </row>
     <row r="32" spans="1:16" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="74" t="s">
+      <c r="A32" s="71" t="s">
         <v>54</v>
       </c>
-      <c r="B32" s="75"/>
-      <c r="C32" s="69" t="s">
+      <c r="B32" s="72"/>
+      <c r="C32" s="66" t="s">
         <v>1</v>
       </c>
-      <c r="D32" s="69"/>
-      <c r="E32" s="69"/>
-      <c r="F32" s="69"/>
-      <c r="G32" s="69"/>
-      <c r="H32" s="69"/>
-      <c r="I32" s="31"/>
-      <c r="J32" s="33"/>
-      <c r="K32" s="31"/>
-      <c r="L32" s="31"/>
-      <c r="M32" s="31"/>
-      <c r="N32" s="31"/>
-      <c r="O32" s="31"/>
-      <c r="P32" s="31"/>
+      <c r="D32" s="66"/>
+      <c r="E32" s="66"/>
+      <c r="F32" s="66"/>
+      <c r="G32" s="66"/>
+      <c r="H32" s="66"/>
+      <c r="I32" s="30"/>
+      <c r="J32" s="32"/>
+      <c r="K32" s="30"/>
+      <c r="L32" s="30"/>
+      <c r="M32" s="30"/>
+      <c r="N32" s="30"/>
+      <c r="O32" s="30"/>
+      <c r="P32" s="30"/>
     </row>
     <row r="33" spans="1:16" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="74" t="s">
+      <c r="A33" s="71" t="s">
         <v>67</v>
       </c>
-      <c r="B33" s="75"/>
-      <c r="C33" s="69" t="s">
+      <c r="B33" s="72"/>
+      <c r="C33" s="66" t="s">
         <v>53</v>
       </c>
-      <c r="D33" s="69"/>
-      <c r="E33" s="69"/>
-      <c r="F33" s="69"/>
-      <c r="G33" s="69"/>
-      <c r="H33" s="69"/>
-      <c r="I33" s="31"/>
-      <c r="J33" s="33"/>
-      <c r="K33" s="31"/>
-      <c r="L33" s="31"/>
-      <c r="M33" s="31"/>
-      <c r="N33" s="31"/>
-      <c r="O33" s="31"/>
-      <c r="P33" s="31"/>
+      <c r="D33" s="66"/>
+      <c r="E33" s="66"/>
+      <c r="F33" s="66"/>
+      <c r="G33" s="66"/>
+      <c r="H33" s="66"/>
+      <c r="I33" s="30"/>
+      <c r="J33" s="32"/>
+      <c r="K33" s="30"/>
+      <c r="L33" s="30"/>
+      <c r="M33" s="30"/>
+      <c r="N33" s="30"/>
+      <c r="O33" s="30"/>
+      <c r="P33" s="30"/>
     </row>
     <row r="34" spans="1:16" s="2" customFormat="1" ht="67.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="38" t="s">
+      <c r="A34" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="B34" s="39"/>
-      <c r="C34" s="39"/>
-      <c r="D34" s="39"/>
-      <c r="E34" s="39"/>
-      <c r="F34" s="39"/>
-      <c r="G34" s="39"/>
-      <c r="H34" s="40"/>
-      <c r="I34" s="31"/>
-      <c r="J34" s="33"/>
-      <c r="K34" s="31"/>
-      <c r="L34" s="31"/>
-      <c r="M34" s="31"/>
-      <c r="N34" s="31"/>
-      <c r="O34" s="31"/>
-      <c r="P34" s="31"/>
+      <c r="B34" s="38"/>
+      <c r="C34" s="38"/>
+      <c r="D34" s="38"/>
+      <c r="E34" s="38"/>
+      <c r="F34" s="38"/>
+      <c r="G34" s="38"/>
+      <c r="H34" s="39"/>
+      <c r="I34" s="30"/>
+      <c r="J34" s="32"/>
+      <c r="K34" s="30"/>
+      <c r="L34" s="30"/>
+      <c r="M34" s="30"/>
+      <c r="N34" s="30"/>
+      <c r="O34" s="30"/>
+      <c r="P34" s="30"/>
     </row>
     <row r="35" spans="1:16" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="88" t="s">
+      <c r="A35" s="85" t="s">
         <v>47</v>
       </c>
-      <c r="B35" s="89"/>
-      <c r="C35" s="89"/>
-      <c r="D35" s="89"/>
-      <c r="E35" s="89"/>
-      <c r="F35" s="89"/>
-      <c r="G35" s="89"/>
-      <c r="H35" s="90"/>
-      <c r="I35" s="31"/>
-      <c r="J35" s="33"/>
-      <c r="K35" s="31"/>
-      <c r="L35" s="31"/>
-      <c r="M35" s="31"/>
-      <c r="N35" s="31"/>
-      <c r="O35" s="31"/>
-      <c r="P35" s="31"/>
+      <c r="B35" s="86"/>
+      <c r="C35" s="86"/>
+      <c r="D35" s="86"/>
+      <c r="E35" s="86"/>
+      <c r="F35" s="86"/>
+      <c r="G35" s="86"/>
+      <c r="H35" s="87"/>
+      <c r="I35" s="30"/>
+      <c r="J35" s="32"/>
+      <c r="K35" s="30"/>
+      <c r="L35" s="30"/>
+      <c r="M35" s="30"/>
+      <c r="N35" s="30"/>
+      <c r="O35" s="30"/>
+      <c r="P35" s="30"/>
     </row>
     <row r="36" spans="1:16" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="79" t="s">
+      <c r="A36" s="76" t="s">
         <v>48</v>
       </c>
-      <c r="B36" s="80"/>
-      <c r="C36" s="80"/>
-      <c r="D36" s="80"/>
-      <c r="E36" s="80"/>
-      <c r="F36" s="80"/>
-      <c r="G36" s="80"/>
-      <c r="H36" s="81"/>
-      <c r="I36" s="31"/>
-      <c r="J36" s="33"/>
-      <c r="K36" s="31"/>
-      <c r="L36" s="31"/>
-      <c r="M36" s="31"/>
-      <c r="N36" s="31"/>
-      <c r="O36" s="31"/>
-      <c r="P36" s="31"/>
+      <c r="B36" s="77"/>
+      <c r="C36" s="77"/>
+      <c r="D36" s="77"/>
+      <c r="E36" s="77"/>
+      <c r="F36" s="77"/>
+      <c r="G36" s="77"/>
+      <c r="H36" s="78"/>
+      <c r="I36" s="30"/>
+      <c r="J36" s="32"/>
+      <c r="K36" s="30"/>
+      <c r="L36" s="30"/>
+      <c r="M36" s="30"/>
+      <c r="N36" s="30"/>
+      <c r="O36" s="30"/>
+      <c r="P36" s="30"/>
     </row>
     <row r="37" spans="1:16" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="82" t="s">
+      <c r="A37" s="79" t="s">
         <v>2</v>
       </c>
-      <c r="B37" s="83"/>
-      <c r="C37" s="83"/>
-      <c r="D37" s="83"/>
-      <c r="E37" s="83"/>
-      <c r="F37" s="83"/>
-      <c r="G37" s="83"/>
-      <c r="H37" s="84"/>
+      <c r="B37" s="80"/>
+      <c r="C37" s="80"/>
+      <c r="D37" s="80"/>
+      <c r="E37" s="80"/>
+      <c r="F37" s="80"/>
+      <c r="G37" s="80"/>
+      <c r="H37" s="81"/>
     </row>
     <row r="38" spans="1:16" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="82" t="s">
+      <c r="A38" s="79" t="s">
         <v>3</v>
       </c>
-      <c r="B38" s="83"/>
-      <c r="C38" s="83"/>
-      <c r="D38" s="83"/>
-      <c r="E38" s="83"/>
-      <c r="F38" s="83"/>
-      <c r="G38" s="83"/>
-      <c r="H38" s="84"/>
+      <c r="B38" s="80"/>
+      <c r="C38" s="80"/>
+      <c r="D38" s="80"/>
+      <c r="E38" s="80"/>
+      <c r="F38" s="80"/>
+      <c r="G38" s="80"/>
+      <c r="H38" s="81"/>
     </row>
     <row r="39" spans="1:16" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A39" s="25"/>
-      <c r="B39" s="26"/>
-      <c r="C39" s="26"/>
-      <c r="D39" s="26"/>
-      <c r="E39" s="26"/>
-      <c r="F39" s="26"/>
-      <c r="G39" s="26"/>
-      <c r="H39" s="27"/>
+      <c r="A39" s="24"/>
+      <c r="B39" s="25"/>
+      <c r="C39" s="25"/>
+      <c r="D39" s="25"/>
+      <c r="E39" s="25"/>
+      <c r="F39" s="25"/>
+      <c r="G39" s="25"/>
+      <c r="H39" s="26"/>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B41" s="28"/>
-      <c r="C41" s="28"/>
-      <c r="D41" s="28"/>
-      <c r="E41" s="28"/>
-      <c r="F41" s="28"/>
-      <c r="G41" s="28"/>
-      <c r="H41" s="28"/>
+      <c r="B41" s="27"/>
+      <c r="C41" s="27"/>
+      <c r="D41" s="27"/>
+      <c r="E41" s="27"/>
+      <c r="F41" s="27"/>
+      <c r="G41" s="27"/>
+      <c r="H41" s="27"/>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B42" s="28"/>
-      <c r="C42" s="28"/>
-      <c r="D42" s="28"/>
-      <c r="E42" s="28"/>
-      <c r="F42" s="28"/>
-      <c r="G42" s="28"/>
-      <c r="H42" s="28"/>
+      <c r="B42" s="27"/>
+      <c r="C42" s="27"/>
+      <c r="D42" s="27"/>
+      <c r="E42" s="27"/>
+      <c r="F42" s="27"/>
+      <c r="G42" s="27"/>
+      <c r="H42" s="27"/>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B43" s="28"/>
-      <c r="C43" s="28"/>
-      <c r="D43" s="28"/>
-      <c r="E43" s="28"/>
-      <c r="F43" s="28"/>
-      <c r="G43" s="28"/>
-      <c r="H43" s="28"/>
+      <c r="B43" s="27"/>
+      <c r="C43" s="27"/>
+      <c r="D43" s="27"/>
+      <c r="E43" s="27"/>
+      <c r="F43" s="27"/>
+      <c r="G43" s="27"/>
+      <c r="H43" s="27"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0"/>

</xml_diff>